<commit_message>
Fastpath for aligned bitreads/writes.
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozidar\Documents\Code\SDR\Ziria\compiler\code\WiFi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimitris\work\ZIRIA\Ziria\code\WiFi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -388,6 +388,15 @@
   </si>
   <si>
     <t>OptRX/Asplos</t>
+  </si>
+  <si>
+    <t>Dimitris</t>
+  </si>
+  <si>
+    <t>DV/SORA</t>
+  </si>
+  <si>
+    <t>2thr/1thr</t>
   </si>
 </sst>
 </file>
@@ -397,7 +406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,8 +443,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +482,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -479,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -508,6 +530,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48:M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,13 +830,15 @@
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>48</v>
       </c>
@@ -847,20 +875,26 @@
       <c r="L1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R1" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -899,24 +933,31 @@
         <f>AVERAGE($I2, $J2, $K2)</f>
         <v>1951.46</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2">
+        <v>2719.83</v>
+      </c>
+      <c r="N2" s="15">
         <f>$H2/$D2</f>
         <v>1.7444714159999812</v>
       </c>
-      <c r="N2" s="15">
+      <c r="O2" s="15">
         <f>$L2/$D2</f>
         <v>1.9566509950899738</v>
       </c>
-      <c r="O2" s="15">
-        <f>$H2/$C2</f>
+      <c r="P2" s="15">
+        <f t="shared" ref="P2:P33" si="0">$H2/$C2</f>
         <v>0.56820487698671884</v>
       </c>
-      <c r="P2" s="15">
+      <c r="Q2" s="15">
         <f>$L2/$C2</f>
         <v>0.63731548007838013</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <f>$M2/$C2</f>
+        <v>0.88825277596342256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
@@ -939,7 +980,7 @@
         <v>2102.1</v>
       </c>
       <c r="H3" s="15">
-        <f t="shared" ref="H3:H66" si="0">AVERAGE($E3, $F3, $G3)</f>
+        <f t="shared" ref="H3:H66" si="1">AVERAGE($E3, $F3, $G3)</f>
         <v>2014.4466666666667</v>
       </c>
       <c r="I3">
@@ -952,27 +993,34 @@
         <v>1834.33</v>
       </c>
       <c r="L3" s="15">
-        <f t="shared" ref="L3:L66" si="1">AVERAGE($I3, $J3, $K3)</f>
+        <f t="shared" ref="L3:L66" si="2">AVERAGE($I3, $J3, $K3)</f>
         <v>1839.7633333333333</v>
       </c>
-      <c r="M3" s="15">
-        <f t="shared" ref="M3:M66" si="2">$H3/$D3</f>
+      <c r="M3">
+        <v>2640.52</v>
+      </c>
+      <c r="N3" s="15">
+        <f t="shared" ref="N3:N66" si="3">$H3/$D3</f>
         <v>3.7567190389606351</v>
       </c>
-      <c r="N3" s="15">
-        <f t="shared" ref="N3:N66" si="3">$L3/$D3</f>
+      <c r="O3" s="15">
+        <f t="shared" ref="O3:O66" si="4">$L3/$D3</f>
         <v>3.4309540460316716</v>
       </c>
-      <c r="O3" s="15">
-        <f>$H3/$C3</f>
+      <c r="P3" s="15">
+        <f t="shared" si="0"/>
         <v>0.77807905240118447</v>
       </c>
-      <c r="P3" s="15">
-        <f t="shared" ref="P3:P48" si="4">$L3/$C3</f>
+      <c r="Q3" s="15">
+        <f t="shared" ref="Q3:Q48" si="5">$L3/$C3</f>
         <v>0.71060769924037592</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <f t="shared" ref="R3:R48" si="6">$M3/$C3</f>
+        <v>1.0198995751255311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -995,7 +1043,7 @@
         <v>4261.12</v>
       </c>
       <c r="H4" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3359.6966666666667</v>
       </c>
       <c r="I4">
@@ -1008,27 +1056,34 @@
         <v>1569.95</v>
       </c>
       <c r="L4" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1572.5033333333333</v>
       </c>
-      <c r="M4" s="15">
-        <f t="shared" si="2"/>
+      <c r="M4">
+        <v>2157.42</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" si="3"/>
         <v>4.3611864363510016</v>
       </c>
-      <c r="N4" s="15">
-        <f t="shared" si="3"/>
+      <c r="O4" s="15">
+        <f t="shared" si="4"/>
         <v>2.0412498177266212</v>
       </c>
-      <c r="O4" s="15">
-        <f>$H4/$C4</f>
+      <c r="P4" s="15">
+        <f t="shared" si="0"/>
         <v>0.90265896471431128</v>
       </c>
-      <c r="P4" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q4" s="15">
+        <f t="shared" si="5"/>
         <v>0.42248880530180905</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <f t="shared" si="6"/>
+        <v>0.57963997850617954</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1106,7 @@
         <v>172.89599999999999</v>
       </c>
       <c r="H5" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>172.9193333333333</v>
       </c>
       <c r="I5">
@@ -1064,27 +1119,34 @@
         <v>171.471</v>
       </c>
       <c r="L5" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>171.79066666666668</v>
       </c>
-      <c r="M5" s="15">
-        <f t="shared" si="2"/>
+      <c r="M5">
+        <v>158.17599999999999</v>
+      </c>
+      <c r="N5" s="15">
+        <f t="shared" si="3"/>
         <v>1.01160870116321</v>
       </c>
-      <c r="N5" s="15">
-        <f t="shared" si="3"/>
+      <c r="O5" s="15">
+        <f t="shared" si="4"/>
         <v>1.0050058014254932</v>
       </c>
-      <c r="O5" s="15">
-        <f>$H5/$C5</f>
+      <c r="P5" s="15">
+        <f t="shared" si="0"/>
         <v>0.83535909822866328</v>
       </c>
-      <c r="P5" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q5" s="15">
+        <f t="shared" si="5"/>
         <v>0.82990660225442836</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <f t="shared" si="6"/>
+        <v>0.76413526570048307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1169,7 @@
         <v>1950.98</v>
       </c>
       <c r="H6" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3590.1966666666667</v>
       </c>
       <c r="I6">
@@ -1120,27 +1182,34 @@
         <v>6271.64</v>
       </c>
       <c r="L6" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6392.77</v>
       </c>
-      <c r="M6" s="15">
-        <f t="shared" si="2"/>
+      <c r="M6">
+        <v>5177.22</v>
+      </c>
+      <c r="N6" s="15">
+        <f t="shared" si="3"/>
         <v>16.858074371808957</v>
       </c>
-      <c r="N6" s="15">
-        <f t="shared" si="3"/>
+      <c r="O6" s="15">
+        <f t="shared" si="4"/>
         <v>30.017796267948874</v>
       </c>
-      <c r="O6" s="15">
-        <f>$H6/$C6</f>
+      <c r="P6" s="15">
+        <f t="shared" si="0"/>
         <v>1.7720615333991445</v>
       </c>
-      <c r="P6" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q6" s="15">
+        <f t="shared" si="5"/>
         <v>3.1553652517275421</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <f t="shared" si="6"/>
+        <v>2.5553899308983219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1163,7 +1232,7 @@
         <v>1957.97</v>
       </c>
       <c r="H7" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2195.4</v>
       </c>
       <c r="I7">
@@ -1176,27 +1245,34 @@
         <v>4430.72</v>
       </c>
       <c r="L7" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4522.7000000000007</v>
       </c>
-      <c r="M7" s="15">
-        <f t="shared" si="2"/>
+      <c r="M7">
+        <v>4259.9399999999996</v>
+      </c>
+      <c r="N7" s="15">
+        <f t="shared" si="3"/>
         <v>9.099047571680801</v>
       </c>
-      <c r="N7" s="15">
-        <f t="shared" si="3"/>
+      <c r="O7" s="15">
+        <f t="shared" si="4"/>
         <v>18.744767446679766</v>
       </c>
-      <c r="O7" s="15">
-        <f>$H7/$C7</f>
+      <c r="P7" s="15">
+        <f t="shared" si="0"/>
         <v>1.5427969079409698</v>
       </c>
-      <c r="P7" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q7" s="15">
+        <f t="shared" si="5"/>
         <v>3.1782853127196069</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <f t="shared" si="6"/>
+        <v>2.9936331693605056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1295,7 @@
         <v>1837.99</v>
       </c>
       <c r="H8" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2411.3866666666668</v>
       </c>
       <c r="I8">
@@ -1232,27 +1308,34 @@
         <v>3501.78</v>
       </c>
       <c r="L8" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3503.8700000000003</v>
       </c>
-      <c r="M8" s="15">
-        <f t="shared" si="2"/>
+      <c r="M8">
+        <v>3202.3</v>
+      </c>
+      <c r="N8" s="15">
+        <f t="shared" si="3"/>
         <v>7.8657994254635772</v>
       </c>
-      <c r="N8" s="15">
-        <f t="shared" si="3"/>
+      <c r="O8" s="15">
+        <f t="shared" si="4"/>
         <v>11.429414873143143</v>
       </c>
-      <c r="O8" s="15">
-        <f>$H8/$C8</f>
+      <c r="P8" s="15">
+        <f t="shared" si="0"/>
         <v>0.49332787779596293</v>
       </c>
-      <c r="P8" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q8" s="15">
+        <f t="shared" si="5"/>
         <v>0.71683101472995092</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <f t="shared" si="6"/>
+        <v>0.65513502454991823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
@@ -1275,7 +1358,7 @@
         <v>2976.7</v>
       </c>
       <c r="H9" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3318.8366666666661</v>
       </c>
       <c r="I9">
@@ -1288,27 +1371,34 @@
         <v>4137.04</v>
       </c>
       <c r="L9" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4516.1400000000003</v>
       </c>
-      <c r="M9" s="15">
-        <f t="shared" si="2"/>
+      <c r="M9">
+        <v>3843.86</v>
+      </c>
+      <c r="N9" s="15">
+        <f t="shared" si="3"/>
         <v>13.281137242504396</v>
       </c>
-      <c r="N9" s="15">
-        <f t="shared" si="3"/>
+      <c r="O9" s="15">
+        <f t="shared" si="4"/>
         <v>18.072439583658475</v>
       </c>
-      <c r="O9" s="15">
-        <f>$H9/$C9</f>
+      <c r="P9" s="15">
+        <f t="shared" si="0"/>
         <v>0.8722303985983354</v>
       </c>
-      <c r="P9" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q9" s="15">
+        <f t="shared" si="5"/>
         <v>1.1868961892247045</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <f t="shared" si="6"/>
+        <v>1.0102128777923784</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -1331,7 +1421,7 @@
         <v>3493.83</v>
       </c>
       <c r="H10" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3420.7766666666666</v>
       </c>
       <c r="I10">
@@ -1344,27 +1434,34 @@
         <v>2892.37</v>
       </c>
       <c r="L10" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2955.64</v>
       </c>
-      <c r="M10" s="15">
-        <f t="shared" si="2"/>
+      <c r="M10">
+        <v>2572.35</v>
+      </c>
+      <c r="N10" s="15">
+        <f t="shared" si="3"/>
         <v>1.3791563522205288</v>
       </c>
-      <c r="N10" s="15">
-        <f t="shared" si="3"/>
+      <c r="O10" s="15">
+        <f t="shared" si="4"/>
         <v>1.1916269543691589</v>
       </c>
-      <c r="O10" s="15">
-        <f>$H10/$C10</f>
+      <c r="P10" s="15">
+        <f t="shared" si="0"/>
         <v>4.5069521299956081</v>
       </c>
-      <c r="P10" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q10" s="15">
+        <f t="shared" si="5"/>
         <v>3.8941238471673252</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <f t="shared" si="6"/>
+        <v>3.3891304347826088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1484,7 @@
         <v>1571.2</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1748.3133333333333</v>
       </c>
       <c r="I11">
@@ -1400,27 +1497,34 @@
         <v>2083.71</v>
       </c>
       <c r="L11" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2095.0700000000002</v>
       </c>
-      <c r="M11" s="15">
-        <f t="shared" si="2"/>
+      <c r="M11">
+        <v>3164.98</v>
+      </c>
+      <c r="N11" s="15">
+        <f t="shared" si="3"/>
         <v>1.9210461158896688</v>
       </c>
-      <c r="N11" s="15">
-        <f t="shared" si="3"/>
+      <c r="O11" s="15">
+        <f t="shared" si="4"/>
         <v>2.302062227222982</v>
       </c>
-      <c r="O11" s="15">
-        <f>$H11/$C11</f>
+      <c r="P11" s="15">
+        <f t="shared" si="0"/>
         <v>0.59812293305964193</v>
       </c>
-      <c r="P11" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q11" s="15">
+        <f t="shared" si="5"/>
         <v>0.71675333561409516</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <f t="shared" si="6"/>
+        <v>1.0827848101265822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
@@ -1443,7 +1547,7 @@
         <v>2681.47</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2827.8333333333335</v>
       </c>
       <c r="I12">
@@ -1456,27 +1560,34 @@
         <v>3120.03</v>
       </c>
       <c r="L12" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3074.5966666666668</v>
       </c>
-      <c r="M12" s="15">
-        <f t="shared" si="2"/>
+      <c r="M12">
+        <v>4280.46</v>
+      </c>
+      <c r="N12" s="15">
+        <f t="shared" si="3"/>
         <v>2.0503134621984409</v>
       </c>
-      <c r="N12" s="15">
-        <f t="shared" si="3"/>
+      <c r="O12" s="15">
+        <f t="shared" si="4"/>
         <v>2.2292285978064896</v>
       </c>
-      <c r="O12" s="15">
-        <f>$H12/$C12</f>
+      <c r="P12" s="15">
+        <f t="shared" si="0"/>
         <v>1.0113853123509777</v>
       </c>
-      <c r="P12" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q12" s="15">
+        <f t="shared" si="5"/>
         <v>1.0996411540295661</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <f t="shared" si="6"/>
+        <v>1.530922746781116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1610,7 @@
         <v>3136.92</v>
       </c>
       <c r="H13" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2737.0433333333335</v>
       </c>
       <c r="I13">
@@ -1512,27 +1623,34 @@
         <v>1953.2</v>
       </c>
       <c r="L13" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1956.9366666666665</v>
       </c>
-      <c r="M13" s="15">
-        <f t="shared" si="2"/>
+      <c r="M13">
+        <v>2291.35</v>
+      </c>
+      <c r="N13" s="15">
+        <f t="shared" si="3"/>
         <v>2.8701463713024862</v>
       </c>
-      <c r="N13" s="15">
-        <f t="shared" si="3"/>
+      <c r="O13" s="15">
+        <f t="shared" si="4"/>
         <v>2.0521029405339273</v>
       </c>
-      <c r="O13" s="15">
-        <f>$H13/$C13</f>
+      <c r="P13" s="15">
+        <f t="shared" si="0"/>
         <v>0.95367363530778171</v>
       </c>
-      <c r="P13" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q13" s="15">
+        <f t="shared" si="5"/>
         <v>0.68185946573751444</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <f t="shared" si="6"/>
+        <v>0.7983797909407665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
@@ -1555,7 +1673,7 @@
         <v>6352.11</v>
       </c>
       <c r="H14" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4850.12</v>
       </c>
       <c r="I14">
@@ -1568,27 +1686,34 @@
         <v>1951.17</v>
       </c>
       <c r="L14" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1962.3033333333333</v>
       </c>
-      <c r="M14" s="15">
-        <f t="shared" si="2"/>
+      <c r="M14">
+        <v>2792.13</v>
+      </c>
+      <c r="N14" s="15">
+        <f t="shared" si="3"/>
         <v>6.5117228249705637</v>
       </c>
-      <c r="N14" s="15">
-        <f t="shared" si="3"/>
+      <c r="O14" s="15">
+        <f t="shared" si="4"/>
         <v>2.634568918950972</v>
       </c>
-      <c r="O14" s="15">
-        <f>$H14/$C14</f>
+      <c r="P14" s="15">
+        <f t="shared" si="0"/>
         <v>1.2803907074973599</v>
       </c>
-      <c r="P14" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q14" s="15">
+        <f t="shared" si="5"/>
         <v>0.51803150299190426</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <f t="shared" si="6"/>
+        <v>0.73709873284054916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1736,7 @@
         <v>1968.38</v>
       </c>
       <c r="H15" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1856.1966666666667</v>
       </c>
       <c r="I15">
@@ -1623,28 +1748,35 @@
       <c r="K15">
         <v>1625.22</v>
       </c>
-      <c r="L15" s="15">
-        <f t="shared" si="1"/>
+      <c r="L15" s="18">
+        <f t="shared" si="2"/>
         <v>1634.82</v>
       </c>
-      <c r="M15" s="15">
-        <f t="shared" si="2"/>
+      <c r="M15">
+        <v>2777.48</v>
+      </c>
+      <c r="N15" s="15">
+        <f t="shared" si="3"/>
         <v>1.8075729541987209</v>
       </c>
-      <c r="N15" s="15">
-        <f t="shared" si="3"/>
+      <c r="O15" s="15">
+        <f t="shared" si="4"/>
         <v>1.5919953257376569</v>
       </c>
-      <c r="O15" s="15">
-        <f>$H15/$C15</f>
+      <c r="P15" s="15">
+        <f t="shared" si="0"/>
         <v>0.49092744423873758</v>
       </c>
-      <c r="P15" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q15" s="15">
+        <f t="shared" si="5"/>
         <v>0.43237767786299919</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <f t="shared" si="6"/>
+        <v>0.73458873313938111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -1667,7 +1799,7 @@
         <v>145.13300000000001</v>
       </c>
       <c r="H16" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>145.46266666666668</v>
       </c>
       <c r="I16">
@@ -1680,27 +1812,34 @@
         <v>145.55699999999999</v>
       </c>
       <c r="L16" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146.26133333333334</v>
       </c>
-      <c r="M16" s="15">
-        <f t="shared" si="2"/>
+      <c r="M16">
+        <v>134.91999999999999</v>
+      </c>
+      <c r="N16" s="15">
+        <f t="shared" si="3"/>
         <v>1.0653171627216624</v>
       </c>
-      <c r="N16" s="15">
-        <f t="shared" si="3"/>
+      <c r="O16" s="15">
+        <f t="shared" si="4"/>
         <v>1.0711663151316304</v>
       </c>
-      <c r="O16" s="15">
-        <f>$H16/$C16</f>
+      <c r="P16" s="15">
+        <f t="shared" si="0"/>
         <v>0.75369257340241802</v>
       </c>
-      <c r="P16" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q16" s="15">
+        <f t="shared" si="5"/>
         <v>0.75783074265975825</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <f t="shared" si="6"/>
+        <v>0.69906735751295335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>20</v>
       </c>
@@ -1723,7 +1862,7 @@
         <v>1147.29</v>
       </c>
       <c r="H17" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1199.2933333333333</v>
       </c>
       <c r="I17">
@@ -1736,27 +1875,34 @@
         <v>1096.94</v>
       </c>
       <c r="L17" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1151.3399999999999</v>
       </c>
-      <c r="M17" s="15">
-        <f t="shared" si="2"/>
+      <c r="M17">
+        <v>1217.3599999999999</v>
+      </c>
+      <c r="N17" s="15">
+        <f t="shared" si="3"/>
         <v>0.8796600555490357</v>
       </c>
-      <c r="N17" s="15">
-        <f t="shared" si="3"/>
+      <c r="O17" s="15">
+        <f t="shared" si="4"/>
         <v>0.84448714939561087</v>
       </c>
-      <c r="O17" s="15">
-        <f>$H17/$C17</f>
+      <c r="P17" s="15">
+        <f t="shared" si="0"/>
         <v>0.71386507936507937</v>
       </c>
-      <c r="P17" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q17" s="15">
+        <f t="shared" si="5"/>
         <v>0.68532142857142853</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <f t="shared" si="6"/>
+        <v>0.72461904761904761</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>28</v>
       </c>
@@ -1779,7 +1925,7 @@
         <v>2084.9</v>
       </c>
       <c r="H18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2049.603333333333</v>
       </c>
       <c r="I18">
@@ -1792,27 +1938,34 @@
         <v>2370.7399999999998</v>
       </c>
       <c r="L18" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2193.8166666666666</v>
       </c>
-      <c r="M18" s="15">
-        <f t="shared" si="2"/>
+      <c r="M18">
+        <v>2149.61</v>
+      </c>
+      <c r="N18" s="15">
+        <f t="shared" si="3"/>
         <v>0.571920611357286</v>
       </c>
-      <c r="N18" s="15">
-        <f t="shared" si="3"/>
+      <c r="O18" s="15">
+        <f t="shared" si="4"/>
         <v>0.61216185044218485</v>
       </c>
-      <c r="O18" s="15">
-        <f>$H18/$C18</f>
+      <c r="P18" s="15">
+        <f t="shared" si="0"/>
         <v>0.42923630017452002</v>
       </c>
-      <c r="P18" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q18" s="15">
+        <f t="shared" si="5"/>
         <v>0.45943804537521815</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <f t="shared" si="6"/>
+        <v>0.4501801047120419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>22</v>
       </c>
@@ -1835,7 +1988,7 @@
         <v>1586.47</v>
       </c>
       <c r="H19" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1483.2333333333333</v>
       </c>
       <c r="I19">
@@ -1848,27 +2001,34 @@
         <v>1780.85</v>
       </c>
       <c r="L19" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1664.3166666666666</v>
       </c>
-      <c r="M19" s="15">
-        <f t="shared" si="2"/>
+      <c r="M19">
+        <v>1447.7</v>
+      </c>
+      <c r="N19" s="15">
+        <f t="shared" si="3"/>
         <v>0.6464214167316763</v>
       </c>
-      <c r="N19" s="15">
-        <f t="shared" si="3"/>
+      <c r="O19" s="15">
+        <f t="shared" si="4"/>
         <v>0.72534099212765424</v>
       </c>
-      <c r="O19" s="15">
-        <f>$H19/$C19</f>
+      <c r="P19" s="15">
+        <f t="shared" si="0"/>
         <v>0.50398686147921623</v>
       </c>
-      <c r="P19" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q19" s="15">
+        <f t="shared" si="5"/>
         <v>0.56551704609808584</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <f t="shared" si="6"/>
+        <v>0.49191301393136255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
@@ -1891,7 +2051,7 @@
         <v>1527.3</v>
       </c>
       <c r="H20" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1764.5966666666666</v>
       </c>
       <c r="I20">
@@ -1904,27 +2064,34 @@
         <v>1570.25</v>
       </c>
       <c r="L20" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1698.2466666666667</v>
       </c>
-      <c r="M20" s="15">
-        <f t="shared" si="2"/>
+      <c r="M20">
+        <v>1523.39</v>
+      </c>
+      <c r="N20" s="15">
+        <f t="shared" si="3"/>
         <v>0.74614228852355502</v>
       </c>
-      <c r="N20" s="15">
-        <f t="shared" si="3"/>
+      <c r="O20" s="15">
+        <f t="shared" si="4"/>
         <v>0.71808684572536818</v>
       </c>
-      <c r="O20" s="15">
-        <f>$H20/$C20</f>
+      <c r="P20" s="15">
+        <f t="shared" si="0"/>
         <v>0.53278884863123988</v>
       </c>
-      <c r="P20" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q20" s="15">
+        <f t="shared" si="5"/>
         <v>0.5127556360708535</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <f t="shared" si="6"/>
+        <v>0.45996074879227056</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1947,7 +2114,7 @@
         <v>1733.4</v>
       </c>
       <c r="H21" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1828.1566666666665</v>
       </c>
       <c r="I21">
@@ -1960,27 +2127,34 @@
         <v>1712.77</v>
       </c>
       <c r="L21" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1701.33</v>
       </c>
-      <c r="M21" s="15">
-        <f t="shared" si="2"/>
+      <c r="M21">
+        <v>1537.28</v>
+      </c>
+      <c r="N21" s="15">
+        <f t="shared" si="3"/>
         <v>0.69826543525810947</v>
       </c>
-      <c r="N21" s="15">
-        <f t="shared" si="3"/>
+      <c r="O21" s="15">
+        <f t="shared" si="4"/>
         <v>0.64982392079873497</v>
       </c>
-      <c r="O21" s="15">
-        <f>$H21/$C21</f>
+      <c r="P21" s="15">
+        <f t="shared" si="0"/>
         <v>0.54328578504210001</v>
       </c>
-      <c r="P21" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q21" s="15">
+        <f t="shared" si="5"/>
         <v>0.50559583952451703</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <f t="shared" si="6"/>
+        <v>0.45684398216939076</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>15</v>
       </c>
@@ -2003,7 +2177,7 @@
         <v>1579.4</v>
       </c>
       <c r="H22" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1788.0466666666664</v>
       </c>
       <c r="I22">
@@ -2016,27 +2190,34 @@
         <v>1531.58</v>
       </c>
       <c r="L22" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1672.6033333333332</v>
       </c>
-      <c r="M22" s="15">
-        <f t="shared" si="2"/>
+      <c r="M22">
+        <v>1714.18</v>
+      </c>
+      <c r="N22" s="15">
+        <f t="shared" si="3"/>
         <v>0.75008564792480314</v>
       </c>
-      <c r="N22" s="15">
-        <f t="shared" si="3"/>
+      <c r="O22" s="15">
+        <f t="shared" si="4"/>
         <v>0.70165716499076403</v>
       </c>
-      <c r="O22" s="15">
-        <f>$H22/$C22</f>
+      <c r="P22" s="15">
+        <f t="shared" si="0"/>
         <v>0.57290825590088634</v>
       </c>
-      <c r="P22" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q22" s="15">
+        <f t="shared" si="5"/>
         <v>0.53591904304176008</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <f t="shared" si="6"/>
+        <v>0.54924062800384499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -2059,7 +2240,7 @@
         <v>1320.34</v>
       </c>
       <c r="H23" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1329.7133333333334</v>
       </c>
       <c r="I23">
@@ -2072,27 +2253,34 @@
         <v>1326.35</v>
       </c>
       <c r="L23" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1343.1666666666667</v>
       </c>
-      <c r="M23" s="15">
-        <f t="shared" si="2"/>
+      <c r="M23">
+        <v>1350.06</v>
+      </c>
+      <c r="N23" s="15">
+        <f t="shared" si="3"/>
         <v>0.76911835022288033</v>
       </c>
-      <c r="N23" s="15">
-        <f t="shared" si="3"/>
+      <c r="O23" s="15">
+        <f t="shared" si="4"/>
         <v>0.77689988123332254</v>
       </c>
-      <c r="O23" s="15">
-        <f>$H23/$C23</f>
+      <c r="P23" s="15">
+        <f t="shared" si="0"/>
         <v>1.5354657428791378</v>
       </c>
-      <c r="P23" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q23" s="15">
+        <f t="shared" si="5"/>
         <v>1.5510007698229409</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <f t="shared" si="6"/>
+        <v>1.5589607390300231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>23</v>
       </c>
@@ -2115,7 +2303,7 @@
         <v>665.57100000000003</v>
       </c>
       <c r="H24" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>604.19666666666672</v>
       </c>
       <c r="I24">
@@ -2128,27 +2316,34 @@
         <v>586.95799999999997</v>
       </c>
       <c r="L24" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>593.75900000000001</v>
       </c>
-      <c r="M24" s="15">
-        <f t="shared" si="2"/>
+      <c r="M24">
+        <v>485.59699999999998</v>
+      </c>
+      <c r="N24" s="15">
+        <f t="shared" si="3"/>
         <v>0.92782898286327387</v>
       </c>
-      <c r="N24" s="15">
-        <f t="shared" si="3"/>
+      <c r="O24" s="15">
+        <f t="shared" si="4"/>
         <v>0.91180047727712488</v>
       </c>
-      <c r="O24" s="15">
-        <f>$H24/$C24</f>
+      <c r="P24" s="15">
+        <f t="shared" si="0"/>
         <v>0.95449710373881003</v>
       </c>
-      <c r="P24" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q24" s="15">
+        <f t="shared" si="5"/>
         <v>0.93800789889415481</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <f t="shared" si="6"/>
+        <v>0.76713586097946285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
@@ -2171,7 +2366,7 @@
         <v>460.505</v>
       </c>
       <c r="H25" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>430.94900000000001</v>
       </c>
       <c r="I25">
@@ -2184,27 +2379,34 @@
         <v>432.97500000000002</v>
       </c>
       <c r="L25" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>431.15200000000004</v>
       </c>
-      <c r="M25" s="15">
-        <f t="shared" si="2"/>
+      <c r="M25">
+        <v>381.79899999999998</v>
+      </c>
+      <c r="N25" s="15">
+        <f t="shared" si="3"/>
         <v>0.94596807473812683</v>
       </c>
-      <c r="N25" s="15">
-        <f t="shared" si="3"/>
+      <c r="O25" s="15">
+        <f t="shared" si="4"/>
         <v>0.94641367623429429</v>
       </c>
-      <c r="O25" s="15">
-        <f>$H25/$C25</f>
+      <c r="P25" s="15">
+        <f t="shared" si="0"/>
         <v>0.82557279693486596</v>
       </c>
-      <c r="P25" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q25" s="15">
+        <f t="shared" si="5"/>
         <v>0.82596168582375484</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <f t="shared" si="6"/>
+        <v>0.73141570881226048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>25</v>
       </c>
@@ -2227,7 +2429,7 @@
         <v>865.83799999999997</v>
       </c>
       <c r="H26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>880.50800000000015</v>
       </c>
       <c r="I26">
@@ -2240,27 +2442,34 @@
         <v>867.17499999999995</v>
       </c>
       <c r="L26" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>872.09833333333336</v>
       </c>
-      <c r="M26" s="15">
-        <f t="shared" si="2"/>
+      <c r="M26">
+        <v>794.90599999999995</v>
+      </c>
+      <c r="N26" s="15">
+        <f t="shared" si="3"/>
         <v>0.88974443700050232</v>
       </c>
-      <c r="N26" s="15">
-        <f t="shared" si="3"/>
+      <c r="O26" s="15">
+        <f t="shared" si="4"/>
         <v>0.88124655380841854</v>
       </c>
-      <c r="O26" s="15">
-        <f>$H26/$C26</f>
+      <c r="P26" s="15">
+        <f t="shared" si="0"/>
         <v>1.1570407358738504</v>
       </c>
-      <c r="P26" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q26" s="15">
+        <f t="shared" si="5"/>
         <v>1.1459899255365746</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <f t="shared" si="6"/>
+        <v>1.0445545335085413</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>18</v>
       </c>
@@ -2283,7 +2492,7 @@
         <v>2604.64</v>
       </c>
       <c r="H27" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2766.3466666666664</v>
       </c>
       <c r="I27">
@@ -2296,27 +2505,34 @@
         <v>2476.7199999999998</v>
       </c>
       <c r="L27" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2675.4033333333332</v>
       </c>
-      <c r="M27" s="15">
-        <f t="shared" si="2"/>
+      <c r="M27">
+        <v>3131.85</v>
+      </c>
+      <c r="N27" s="15">
+        <f t="shared" si="3"/>
         <v>0.67114363164670787</v>
       </c>
-      <c r="N27" s="15">
-        <f t="shared" si="3"/>
+      <c r="O27" s="15">
+        <f t="shared" si="4"/>
         <v>0.64907986077415258</v>
       </c>
-      <c r="O27" s="15">
-        <f>$H27/$C27</f>
+      <c r="P27" s="15">
+        <f t="shared" si="0"/>
         <v>2.4287503658179688</v>
       </c>
-      <c r="P27" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q27" s="15">
+        <f t="shared" si="5"/>
         <v>2.3489054726368157</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <f t="shared" si="6"/>
+        <v>2.7496488147497806</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>24</v>
       </c>
@@ -2339,7 +2555,7 @@
         <v>400.726</v>
       </c>
       <c r="H28" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>381.73466666666673</v>
       </c>
       <c r="I28">
@@ -2352,27 +2568,34 @@
         <v>400.39600000000002</v>
       </c>
       <c r="L28" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>385.73133333333334</v>
       </c>
-      <c r="M28" s="15">
-        <f t="shared" si="2"/>
+      <c r="M28">
+        <v>409.375</v>
+      </c>
+      <c r="N28" s="15">
+        <f t="shared" si="3"/>
         <v>0.98748659154482665</v>
       </c>
-      <c r="N28" s="15">
-        <f t="shared" si="3"/>
+      <c r="O28" s="15">
+        <f t="shared" si="4"/>
         <v>0.99782532964967285</v>
       </c>
-      <c r="O28" s="15">
-        <f>$H28/$C28</f>
+      <c r="P28" s="15">
+        <f t="shared" si="0"/>
         <v>0.82093476702508972</v>
       </c>
-      <c r="P28" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q28" s="15">
+        <f t="shared" si="5"/>
         <v>0.82952974910394262</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <f t="shared" si="6"/>
+        <v>0.8803763440860215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>16</v>
       </c>
@@ -2395,7 +2618,7 @@
         <v>189.374</v>
       </c>
       <c r="H29" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189.30233333333334</v>
       </c>
       <c r="I29">
@@ -2408,27 +2631,34 @@
         <v>145.52000000000001</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144.77933333333331</v>
       </c>
-      <c r="M29" s="15">
-        <f t="shared" si="2"/>
+      <c r="M29">
+        <v>135.744</v>
+      </c>
+      <c r="N29" s="15">
+        <f t="shared" si="3"/>
         <v>0.8908303176612502</v>
       </c>
-      <c r="N29" s="15">
-        <f t="shared" si="3"/>
+      <c r="O29" s="15">
+        <f t="shared" si="4"/>
         <v>0.68131130363308079</v>
       </c>
-      <c r="O29" s="15">
-        <f>$H29/$C29</f>
+      <c r="P29" s="15">
+        <f t="shared" si="0"/>
         <v>0.52006135531135533</v>
       </c>
-      <c r="P29" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q29" s="15">
+        <f t="shared" si="5"/>
         <v>0.39774542124542117</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <f t="shared" si="6"/>
+        <v>0.37292307692307691</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>26</v>
       </c>
@@ -2451,7 +2681,7 @@
         <v>273.529</v>
       </c>
       <c r="H30" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>273.80333333333334</v>
       </c>
       <c r="I30">
@@ -2464,27 +2694,34 @@
         <v>276.07499999999999</v>
       </c>
       <c r="L30" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>276.70033333333339</v>
       </c>
-      <c r="M30" s="15">
-        <f t="shared" si="2"/>
+      <c r="M30">
+        <v>259.03100000000001</v>
+      </c>
+      <c r="N30" s="15">
+        <f t="shared" si="3"/>
         <v>1.0256957763925516</v>
       </c>
-      <c r="N30" s="15">
-        <f t="shared" si="3"/>
+      <c r="O30" s="15">
+        <f t="shared" si="4"/>
         <v>1.0365482398305763</v>
       </c>
-      <c r="O30" s="15">
-        <f>$H30/$C30</f>
+      <c r="P30" s="15">
+        <f t="shared" si="0"/>
         <v>0.62943295019157086</v>
       </c>
-      <c r="P30" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q30" s="15">
+        <f t="shared" si="5"/>
         <v>0.63609272030651354</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <f t="shared" si="6"/>
+        <v>0.59547356321839084</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
@@ -2507,7 +2744,7 @@
         <v>1627.39</v>
       </c>
       <c r="H31" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1350.04</v>
       </c>
       <c r="I31">
@@ -2520,27 +2757,34 @@
         <v>1286.3900000000001</v>
       </c>
       <c r="L31" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1322.1500000000003</v>
       </c>
-      <c r="M31" s="15">
-        <f t="shared" si="2"/>
+      <c r="M31">
+        <v>1197.33</v>
+      </c>
+      <c r="N31" s="15">
+        <f t="shared" si="3"/>
         <v>0.81161476493928097</v>
       </c>
-      <c r="N31" s="15">
-        <f t="shared" si="3"/>
+      <c r="O31" s="15">
+        <f t="shared" si="4"/>
         <v>0.79484790188770005</v>
       </c>
-      <c r="O31" s="15">
-        <f>$H31/$C31</f>
+      <c r="P31" s="15">
+        <f t="shared" si="0"/>
         <v>2.0963354037267079</v>
       </c>
-      <c r="P31" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q31" s="15">
+        <f t="shared" si="5"/>
         <v>2.0530279503105593</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <f t="shared" si="6"/>
+        <v>1.8592080745341615</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>30</v>
       </c>
@@ -2563,7 +2807,7 @@
         <v>111.54900000000001</v>
       </c>
       <c r="H32" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110.04699999999998</v>
       </c>
       <c r="I32">
@@ -2576,27 +2820,34 @@
         <v>116.036</v>
       </c>
       <c r="L32" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.96733333333333</v>
       </c>
-      <c r="M32" s="15">
-        <f t="shared" si="2"/>
+      <c r="M32">
+        <v>105.496</v>
+      </c>
+      <c r="N32" s="15">
+        <f t="shared" si="3"/>
         <v>0.99254108267041852</v>
       </c>
-      <c r="N32" s="15">
-        <f t="shared" si="3"/>
+      <c r="O32" s="15">
+        <f t="shared" si="4"/>
         <v>1.0459380317597753</v>
       </c>
-      <c r="O32" s="15">
-        <f>$H32/$C32</f>
+      <c r="P32" s="15">
+        <f t="shared" si="0"/>
         <v>0.66695151515151507</v>
       </c>
-      <c r="P32" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q32" s="15">
+        <f t="shared" si="5"/>
         <v>0.70283232323232325</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <f t="shared" si="6"/>
+        <v>0.63936969696969692</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>47</v>
       </c>
@@ -2619,7 +2870,7 @@
         <v>119.86499999999999</v>
       </c>
       <c r="H33" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>125.98366666666668</v>
       </c>
       <c r="I33">
@@ -2632,27 +2883,34 @@
         <v>129.76499999999999</v>
       </c>
       <c r="L33" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>129.70066666666665</v>
       </c>
-      <c r="M33" s="15">
-        <f t="shared" si="2"/>
+      <c r="M33">
+        <v>104.913</v>
+      </c>
+      <c r="N33" s="15">
+        <f t="shared" si="3"/>
         <v>1.0616392374307249</v>
       </c>
-      <c r="N33" s="15">
-        <f t="shared" si="3"/>
+      <c r="O33" s="15">
+        <f t="shared" si="4"/>
         <v>1.0929616552483516</v>
       </c>
-      <c r="O33" s="15">
-        <f>$H33/$C33</f>
+      <c r="P33" s="15">
+        <f t="shared" si="0"/>
         <v>0.76819308943089437</v>
       </c>
-      <c r="P33" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q33" s="15">
+        <f t="shared" si="5"/>
         <v>0.79085772357723572</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <f t="shared" si="6"/>
+        <v>0.63971341463414633</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
@@ -2669,7 +2927,7 @@
         <v>108.1</v>
       </c>
       <c r="H34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110.83566666666667</v>
       </c>
       <c r="I34">
@@ -2682,21 +2940,24 @@
         <v>115.73699999999999</v>
       </c>
       <c r="L34" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.44233333333334</v>
       </c>
-      <c r="M34" s="15">
-        <f t="shared" si="2"/>
+      <c r="M34">
+        <v>97.739599999999996</v>
+      </c>
+      <c r="N34" s="15">
+        <f t="shared" si="3"/>
         <v>1.0397634705166814</v>
       </c>
-      <c r="N34" s="15">
-        <f t="shared" si="3"/>
+      <c r="O34" s="15">
+        <f t="shared" si="4"/>
         <v>1.0642169416900413</v>
       </c>
-      <c r="O34" s="15"/>
       <c r="P34" s="15"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="15"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>42</v>
       </c>
@@ -2719,7 +2980,7 @@
         <v>91.206000000000003</v>
       </c>
       <c r="H35" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>91.169533333333334</v>
       </c>
       <c r="I35">
@@ -2732,27 +2993,34 @@
         <v>90.831500000000005</v>
       </c>
       <c r="L35" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.259233333333327</v>
       </c>
-      <c r="M35" s="15">
-        <f t="shared" si="2"/>
+      <c r="M35">
+        <v>78.779799999999994</v>
+      </c>
+      <c r="N35" s="15">
+        <f t="shared" si="3"/>
         <v>1.0699996400845644</v>
       </c>
-      <c r="N35" s="15">
-        <f t="shared" si="3"/>
+      <c r="O35" s="15">
+        <f t="shared" si="4"/>
         <v>1.0475796469386061</v>
       </c>
-      <c r="O35" s="15">
+      <c r="P35" s="15">
         <f>$H35/$C35</f>
         <v>0.72935626666666664</v>
       </c>
-      <c r="P35" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q35" s="15">
+        <f t="shared" si="5"/>
         <v>0.71407386666666661</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <f t="shared" si="6"/>
+        <v>0.63023839999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>44</v>
       </c>
@@ -2769,7 +3037,7 @@
         <v>78.892499999999998</v>
       </c>
       <c r="H36" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>79.048600000000008</v>
       </c>
       <c r="I36">
@@ -2782,21 +3050,24 @@
         <v>78.7851</v>
       </c>
       <c r="L36" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78.144599999999997</v>
       </c>
-      <c r="M36" s="15">
-        <f t="shared" si="2"/>
+      <c r="M36">
+        <v>55.382899999999999</v>
+      </c>
+      <c r="N36" s="15">
+        <f t="shared" si="3"/>
         <v>1.1265619655683503</v>
       </c>
-      <c r="N36" s="15">
-        <f t="shared" si="3"/>
+      <c r="O36" s="15">
+        <f t="shared" si="4"/>
         <v>1.1136785999315926</v>
       </c>
-      <c r="O36" s="15"/>
       <c r="P36" s="15"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q36" s="15"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>43</v>
       </c>
@@ -2819,7 +3090,7 @@
         <v>56.840800000000002</v>
       </c>
       <c r="H37" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57.5563</v>
       </c>
       <c r="I37">
@@ -2832,27 +3103,34 @@
         <v>58.984999999999999</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.412166666666657</v>
       </c>
-      <c r="M37" s="15">
-        <f t="shared" si="2"/>
+      <c r="M37">
+        <v>46.868600000000001</v>
+      </c>
+      <c r="N37" s="15">
+        <f t="shared" si="3"/>
         <v>1.039945433684762</v>
       </c>
-      <c r="N37" s="15">
-        <f t="shared" si="3"/>
+      <c r="O37" s="15">
+        <f t="shared" si="4"/>
         <v>1.0554095033320985</v>
       </c>
-      <c r="O37" s="15">
+      <c r="P37" s="15">
         <f>$H37/$C37</f>
         <v>0.71057160493827165</v>
       </c>
-      <c r="P37" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q37" s="15">
+        <f t="shared" si="5"/>
         <v>0.7211378600823044</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <f t="shared" si="6"/>
+        <v>0.57862469135802475</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>40</v>
       </c>
@@ -2869,7 +3147,7 @@
         <v>48.8964</v>
       </c>
       <c r="H38" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48.727299999999993</v>
       </c>
       <c r="I38">
@@ -2882,21 +3160,24 @@
         <v>49.027900000000002</v>
       </c>
       <c r="L38" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48.98843333333334</v>
       </c>
-      <c r="M38" s="15">
-        <f t="shared" si="2"/>
+      <c r="M38">
+        <v>38.995800000000003</v>
+      </c>
+      <c r="N38" s="15">
+        <f t="shared" si="3"/>
         <v>1.1153576758622581</v>
       </c>
-      <c r="N38" s="15">
-        <f t="shared" si="3"/>
+      <c r="O38" s="15">
+        <f t="shared" si="4"/>
         <v>1.1213349630863982</v>
       </c>
-      <c r="O38" s="15"/>
       <c r="P38" s="15"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38" s="15"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>33</v>
       </c>
@@ -2919,7 +3200,7 @@
         <v>36.943600000000004</v>
       </c>
       <c r="H39" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36.8904</v>
       </c>
       <c r="I39">
@@ -2932,27 +3213,34 @@
         <v>36.532800000000002</v>
       </c>
       <c r="L39" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36.468166666666669</v>
       </c>
-      <c r="M39" s="15">
-        <f t="shared" si="2"/>
+      <c r="M39">
+        <v>30.373999999999999</v>
+      </c>
+      <c r="N39" s="15">
+        <f t="shared" si="3"/>
         <v>1.1129668738309297</v>
       </c>
-      <c r="N39" s="15">
-        <f t="shared" si="3"/>
+      <c r="O39" s="15">
+        <f t="shared" si="4"/>
         <v>1.1002282829501799</v>
       </c>
-      <c r="O39" s="15">
+      <c r="P39" s="15">
         <f>$H39/$C39</f>
         <v>0.60476065573770488</v>
       </c>
-      <c r="P39" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q39" s="15">
+        <f t="shared" si="5"/>
         <v>0.59783879781420768</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <f t="shared" si="6"/>
+        <v>0.49793442622950818</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>37</v>
       </c>
@@ -2969,7 +3257,7 @@
         <v>35.248399999999997</v>
       </c>
       <c r="H40" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35.268400000000007</v>
       </c>
       <c r="I40">
@@ -2982,21 +3270,24 @@
         <v>35.691600000000001</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.565566666666662</v>
       </c>
-      <c r="M40" s="15">
-        <f t="shared" si="2"/>
+      <c r="M40">
+        <v>29.0684</v>
+      </c>
+      <c r="N40" s="15">
+        <f t="shared" si="3"/>
         <v>1.1194505016648102</v>
       </c>
-      <c r="N40" s="15">
-        <f t="shared" si="3"/>
+      <c r="O40" s="15">
+        <f t="shared" si="4"/>
         <v>1.1288828369586721</v>
       </c>
-      <c r="O40" s="15"/>
       <c r="P40" s="15"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40" s="15"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>35</v>
       </c>
@@ -3019,7 +3310,7 @@
         <v>259.72300000000001</v>
       </c>
       <c r="H41" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>259.79400000000004</v>
       </c>
       <c r="I41">
@@ -3032,27 +3323,34 @@
         <v>259.78100000000001</v>
       </c>
       <c r="L41" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260.86233333333331</v>
       </c>
-      <c r="M41" s="15">
-        <f t="shared" si="2"/>
+      <c r="M41">
+        <v>217.18299999999999</v>
+      </c>
+      <c r="N41" s="15">
+        <f t="shared" si="3"/>
         <v>1.0520531303150564</v>
       </c>
-      <c r="N41" s="15">
-        <f t="shared" si="3"/>
+      <c r="O41" s="15">
+        <f t="shared" si="4"/>
         <v>1.0563794174023378</v>
       </c>
-      <c r="O41" s="15">
+      <c r="P41" s="15">
         <f>$H41/$C41</f>
         <v>0.89894117647058835</v>
       </c>
-      <c r="P41" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q41" s="15">
+        <f t="shared" si="5"/>
         <v>0.90263783160322941</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <f t="shared" si="6"/>
+        <v>0.75149826989619373</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>38</v>
       </c>
@@ -3075,7 +3373,7 @@
         <v>50.97</v>
       </c>
       <c r="H42" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51.04593333333333</v>
       </c>
       <c r="I42">
@@ -3088,27 +3386,34 @@
         <v>52.031700000000001</v>
       </c>
       <c r="L42" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52.357100000000003</v>
       </c>
-      <c r="M42" s="15">
-        <f t="shared" si="2"/>
+      <c r="M42">
+        <v>49.960700000000003</v>
+      </c>
+      <c r="N42" s="15">
+        <f t="shared" si="3"/>
         <v>1.4172536498461397</v>
       </c>
-      <c r="N42" s="15">
-        <f t="shared" si="3"/>
+      <c r="O42" s="15">
+        <f t="shared" si="4"/>
         <v>1.4536572499479421</v>
       </c>
-      <c r="O42" s="15">
+      <c r="P42" s="15">
         <f>$H42/$C42</f>
         <v>0.94529506172839506</v>
       </c>
-      <c r="P42" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q42" s="15">
+        <f t="shared" si="5"/>
         <v>0.96957592592592601</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <f t="shared" si="6"/>
+        <v>0.92519814814814816</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>45</v>
       </c>
@@ -3125,7 +3430,7 @@
         <v>69.766000000000005</v>
       </c>
       <c r="H43" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.665366666666671</v>
       </c>
       <c r="I43">
@@ -3138,21 +3443,24 @@
         <v>74.892700000000005</v>
       </c>
       <c r="L43" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74.592966666666669</v>
       </c>
-      <c r="M43" s="15">
-        <f t="shared" si="2"/>
+      <c r="M43">
+        <v>71.829800000000006</v>
+      </c>
+      <c r="N43" s="15">
+        <f t="shared" si="3"/>
         <v>1.5095322601731012</v>
       </c>
-      <c r="N43" s="15">
-        <f t="shared" si="3"/>
+      <c r="O43" s="15">
+        <f t="shared" si="4"/>
         <v>1.6163051305553089</v>
       </c>
-      <c r="O43" s="15"/>
       <c r="P43" s="15"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43" s="15"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>39</v>
       </c>
@@ -3175,7 +3483,7 @@
         <v>91.989699999999999</v>
       </c>
       <c r="H44" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>92.123233333333317</v>
       </c>
       <c r="I44">
@@ -3188,27 +3496,34 @@
         <v>95.262799999999999</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.839200000000005</v>
       </c>
-      <c r="M44" s="15">
-        <f t="shared" si="2"/>
+      <c r="M44">
+        <v>86.194000000000003</v>
+      </c>
+      <c r="N44" s="15">
+        <f t="shared" si="3"/>
         <v>2.0632534145585799</v>
       </c>
-      <c r="N44" s="15">
-        <f t="shared" si="3"/>
+      <c r="O44" s="15">
+        <f t="shared" si="4"/>
         <v>2.1240820165959304</v>
       </c>
-      <c r="O44" s="15">
+      <c r="P44" s="15">
         <f>$H44/$C44</f>
         <v>0.94003299319727873</v>
       </c>
-      <c r="P44" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q44" s="15">
+        <f t="shared" si="5"/>
         <v>0.96774693877551021</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <f t="shared" si="6"/>
+        <v>0.87953061224489804</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>31</v>
       </c>
@@ -3225,7 +3540,7 @@
         <v>116.24299999999999</v>
       </c>
       <c r="H45" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>115.985</v>
       </c>
       <c r="I45">
@@ -3238,21 +3553,24 @@
         <v>127.81</v>
       </c>
       <c r="L45" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127.64966666666668</v>
       </c>
-      <c r="M45" s="15">
-        <f t="shared" si="2"/>
+      <c r="M45">
+        <v>105.68300000000001</v>
+      </c>
+      <c r="N45" s="15">
+        <f t="shared" si="3"/>
         <v>2.0946242462440878</v>
       </c>
-      <c r="N45" s="15">
-        <f t="shared" si="3"/>
+      <c r="O45" s="15">
+        <f t="shared" si="4"/>
         <v>2.3052816038709811</v>
       </c>
-      <c r="O45" s="15"/>
       <c r="P45" s="15"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45" s="15"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>41</v>
       </c>
@@ -3275,7 +3593,7 @@
         <v>149.459</v>
       </c>
       <c r="H46" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>149.32566666666668</v>
       </c>
       <c r="I46">
@@ -3288,27 +3606,34 @@
         <v>157.99299999999999</v>
       </c>
       <c r="L46" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>157.87433333333334</v>
       </c>
-      <c r="M46" s="15">
-        <f t="shared" si="2"/>
+      <c r="M46">
+        <v>151.34299999999999</v>
+      </c>
+      <c r="N46" s="15">
+        <f t="shared" si="3"/>
         <v>2.7538514405288161</v>
       </c>
-      <c r="N46" s="15">
-        <f t="shared" si="3"/>
+      <c r="O46" s="15">
+        <f t="shared" si="4"/>
         <v>2.9115052353526618</v>
       </c>
-      <c r="O46" s="15">
+      <c r="P46" s="15">
         <f>$H46/$C46</f>
         <v>1.029832183908046</v>
       </c>
-      <c r="P46" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q46" s="15">
+        <f t="shared" si="5"/>
         <v>1.0887885057471265</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <f t="shared" si="6"/>
+        <v>1.0437448275862069</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>46</v>
       </c>
@@ -3325,7 +3650,7 @@
         <v>173.72399999999999</v>
       </c>
       <c r="H47" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>172.85133333333332</v>
       </c>
       <c r="I47">
@@ -3338,21 +3663,24 @@
         <v>206.26599999999999</v>
       </c>
       <c r="L47" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>204.95266666666666</v>
       </c>
-      <c r="M47" s="15">
-        <f t="shared" si="2"/>
+      <c r="M47">
+        <v>189.08</v>
+      </c>
+      <c r="N47" s="15">
+        <f t="shared" si="3"/>
         <v>2.6837185375179455</v>
       </c>
-      <c r="N47" s="15">
-        <f t="shared" si="3"/>
+      <c r="O47" s="15">
+        <f t="shared" si="4"/>
         <v>3.1821291756330279</v>
       </c>
-      <c r="O47" s="15"/>
       <c r="P47" s="15"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q47" s="15"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>32</v>
       </c>
@@ -3375,7 +3703,7 @@
         <v>155.672</v>
       </c>
       <c r="H48" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>155.75133333333335</v>
       </c>
       <c r="I48">
@@ -3387,28 +3715,38 @@
       <c r="K48">
         <v>170.68</v>
       </c>
-      <c r="L48" s="15">
-        <f t="shared" si="1"/>
+      <c r="L48" s="20">
+        <f t="shared" si="2"/>
         <v>171.40966666666668</v>
       </c>
-      <c r="M48" s="15">
-        <f t="shared" si="2"/>
+      <c r="M48" s="21">
+        <v>142.33000000000001</v>
+      </c>
+      <c r="N48" s="15">
+        <f t="shared" si="3"/>
         <v>2.8005123290413492</v>
       </c>
-      <c r="N48" s="15">
-        <f t="shared" si="3"/>
+      <c r="O48" s="15">
+        <f t="shared" si="4"/>
         <v>3.0820595531565358</v>
       </c>
-      <c r="O48" s="15">
+      <c r="P48" s="15">
         <f>$H48/$C48</f>
         <v>0.67424819624819632</v>
       </c>
-      <c r="P48" s="15">
-        <f t="shared" si="4"/>
+      <c r="Q48" s="20">
+        <f t="shared" si="5"/>
         <v>0.74203318903318904</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="R48" s="21">
+        <f t="shared" si="6"/>
+        <v>0.61614718614718622</v>
+      </c>
+      <c r="T48" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>34</v>
       </c>
@@ -3425,7 +3763,7 @@
         <v>142.53899999999999</v>
       </c>
       <c r="H49" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>142.05533333333332</v>
       </c>
       <c r="I49">
@@ -3437,20 +3775,23 @@
       <c r="K49">
         <v>177.98599999999999</v>
       </c>
-      <c r="L49" s="15">
-        <f t="shared" si="1"/>
+      <c r="L49" s="20">
+        <f t="shared" si="2"/>
         <v>178.10233333333335</v>
       </c>
-      <c r="M49" s="15">
-        <f t="shared" si="2"/>
+      <c r="M49" s="21">
+        <v>171.405</v>
+      </c>
+      <c r="N49" s="15">
+        <f t="shared" si="3"/>
         <v>2.4140636373472182</v>
       </c>
-      <c r="N49" s="15">
-        <f t="shared" si="3"/>
+      <c r="O49" s="15">
+        <f t="shared" si="4"/>
         <v>3.026640088322579</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>47</v>
       </c>
@@ -3467,7 +3808,7 @@
         <v>185.01300000000001</v>
       </c>
       <c r="H50" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>160.57100000000003</v>
       </c>
       <c r="I50">
@@ -3480,19 +3821,24 @@
         <v>182.14699999999999</v>
       </c>
       <c r="L50" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180.85566666666668</v>
       </c>
-      <c r="M50" s="15">
-        <f t="shared" si="2"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15">
+        <f t="shared" si="3"/>
         <v>0.97979643890116075</v>
       </c>
-      <c r="N50" s="15">
-        <f t="shared" si="3"/>
+      <c r="O50" s="15">
+        <f t="shared" si="4"/>
         <v>1.1035724891486964</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T50" s="20">
+        <f>$L50/$L33</f>
+        <v>1.3944081500480596</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>36</v>
       </c>
@@ -3509,7 +3855,7 @@
         <v>176.494</v>
       </c>
       <c r="H51" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>176.32033333333334</v>
       </c>
       <c r="I51">
@@ -3522,19 +3868,24 @@
         <v>168.285</v>
       </c>
       <c r="L51" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144.90886666666665</v>
       </c>
-      <c r="M51" s="15">
-        <f t="shared" si="2"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15">
+        <f t="shared" si="3"/>
         <v>1.0755830740763335</v>
       </c>
-      <c r="N51" s="15">
-        <f t="shared" si="3"/>
+      <c r="O51" s="15">
+        <f t="shared" si="4"/>
         <v>0.88396795380141924</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T51" s="20">
+        <f t="shared" ref="T51:T66" si="7">$L51/$L34</f>
+        <v>1.2773791089158366</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
@@ -3551,7 +3902,7 @@
         <v>152.68799999999999</v>
       </c>
       <c r="H52" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>152.108</v>
       </c>
       <c r="I52">
@@ -3564,19 +3915,24 @@
         <v>150.65100000000001</v>
       </c>
       <c r="L52" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>154.77833333333334</v>
       </c>
-      <c r="M52" s="15">
-        <f t="shared" si="2"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15">
+        <f t="shared" si="3"/>
         <v>1.172297922190024</v>
       </c>
-      <c r="N52" s="15">
-        <f t="shared" si="3"/>
+      <c r="O52" s="15">
+        <f t="shared" si="4"/>
         <v>1.1928782086852867</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T52" s="15">
+        <f>$L52/$L35</f>
+        <v>1.7340316239925879</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>44</v>
       </c>
@@ -3593,7 +3949,7 @@
         <v>125.282</v>
       </c>
       <c r="H53" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>122.76799999999999</v>
       </c>
       <c r="I53">
@@ -3606,19 +3962,24 @@
         <v>127.078</v>
       </c>
       <c r="L53" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127.551</v>
       </c>
-      <c r="M53" s="15">
-        <f t="shared" si="2"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15">
+        <f t="shared" si="3"/>
         <v>1.1505365259359916</v>
       </c>
-      <c r="N53" s="15">
-        <f t="shared" si="3"/>
+      <c r="O53" s="15">
+        <f t="shared" si="4"/>
         <v>1.1953610421254861</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T53" s="15">
+        <f t="shared" si="7"/>
+        <v>1.6322433028001935</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>43</v>
       </c>
@@ -3635,7 +3996,7 @@
         <v>77.868899999999996</v>
       </c>
       <c r="H54" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>79.312866666666665</v>
       </c>
       <c r="I54">
@@ -3648,19 +4009,24 @@
         <v>85.010099999999994</v>
       </c>
       <c r="L54" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84.682333333333332</v>
       </c>
-      <c r="M54" s="15">
-        <f t="shared" si="2"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15">
+        <f t="shared" si="3"/>
         <v>1.0529057963703432</v>
       </c>
-      <c r="N54" s="15">
-        <f t="shared" si="3"/>
+      <c r="O54" s="15">
+        <f t="shared" si="4"/>
         <v>1.1241873275311218</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T54" s="15">
+        <f t="shared" si="7"/>
+        <v>1.4497379256033991</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>40</v>
       </c>
@@ -3677,7 +4043,7 @@
         <v>64.173100000000005</v>
       </c>
       <c r="H55" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65.45450000000001</v>
       </c>
       <c r="I55">
@@ -3690,19 +4056,24 @@
         <v>67.475999999999999</v>
       </c>
       <c r="L55" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67.298966666666672</v>
       </c>
-      <c r="M55" s="15">
-        <f t="shared" si="2"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15">
+        <f t="shared" si="3"/>
         <v>1.096131399451721</v>
       </c>
-      <c r="N55" s="15">
-        <f t="shared" si="3"/>
+      <c r="O55" s="15">
+        <f t="shared" si="4"/>
         <v>1.1270196932829377</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T55" s="15">
+        <f t="shared" si="7"/>
+        <v>1.373772584412783</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>33</v>
       </c>
@@ -3719,7 +4090,7 @@
         <v>47.824399999999997</v>
       </c>
       <c r="H56" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47.416766666666661</v>
       </c>
       <c r="I56">
@@ -3732,19 +4103,24 @@
         <v>47.047600000000003</v>
       </c>
       <c r="L56" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47.961100000000009</v>
       </c>
-      <c r="M56" s="15">
-        <f t="shared" si="2"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15">
+        <f t="shared" si="3"/>
         <v>1.1068236213169498</v>
       </c>
-      <c r="N56" s="15">
-        <f t="shared" si="3"/>
+      <c r="O56" s="15">
+        <f t="shared" si="4"/>
         <v>1.1195296962680088</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T56" s="15">
+        <f t="shared" si="7"/>
+        <v>1.3151497424694598</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>37</v>
       </c>
@@ -3761,7 +4137,7 @@
         <v>44.664299999999997</v>
       </c>
       <c r="H57" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45.128399999999999</v>
       </c>
       <c r="I57">
@@ -3774,19 +4150,24 @@
         <v>46.227600000000002</v>
       </c>
       <c r="L57" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45.840899999999998</v>
       </c>
-      <c r="M57" s="15">
-        <f t="shared" si="2"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15">
+        <f t="shared" si="3"/>
         <v>1.1306862027840971</v>
       </c>
-      <c r="N57" s="15">
-        <f t="shared" si="3"/>
+      <c r="O57" s="15">
+        <f t="shared" si="4"/>
         <v>1.1485377977771318</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T57" s="15">
+        <f t="shared" si="7"/>
+        <v>1.2889124031015018</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>35</v>
       </c>
@@ -3803,7 +4184,7 @@
         <v>33.998800000000003</v>
       </c>
       <c r="H58" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34.024633333333334</v>
       </c>
       <c r="I58">
@@ -3816,19 +4197,24 @@
         <v>33.927399999999999</v>
       </c>
       <c r="L58" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.00436666666667</v>
       </c>
-      <c r="M58" s="15">
-        <f t="shared" si="2"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15">
+        <f t="shared" si="3"/>
         <v>0.1560970649000708</v>
       </c>
-      <c r="N58" s="15">
-        <f t="shared" si="3"/>
+      <c r="O58" s="15">
+        <f t="shared" si="4"/>
         <v>0.15600408617048447</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T58" s="15">
+        <f t="shared" si="7"/>
+        <v>0.13035368591607069</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>38</v>
       </c>
@@ -3845,7 +4231,7 @@
         <v>49.778799999999997</v>
       </c>
       <c r="H59" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49.125</v>
       </c>
       <c r="I59">
@@ -3858,19 +4244,24 @@
         <v>49.747100000000003</v>
       </c>
       <c r="L59" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49.632033333333332</v>
       </c>
-      <c r="M59" s="15">
-        <f t="shared" si="2"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15">
+        <f t="shared" si="3"/>
         <v>1.0614346491161732</v>
       </c>
-      <c r="N59" s="15">
-        <f t="shared" si="3"/>
+      <c r="O59" s="15">
+        <f t="shared" si="4"/>
         <v>1.0723900231264913</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T59" s="15">
+        <f t="shared" si="7"/>
+        <v>0.94795229936977654</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>45</v>
       </c>
@@ -3887,7 +4278,7 @@
         <v>74.329099999999997</v>
       </c>
       <c r="H60" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>73.173633333333328</v>
       </c>
       <c r="I60">
@@ -3900,19 +4291,24 @@
         <v>73.7149</v>
       </c>
       <c r="L60" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73.19</v>
       </c>
-      <c r="M60" s="15">
-        <f t="shared" si="2"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15">
+        <f t="shared" si="3"/>
         <v>1.2383839922375663</v>
       </c>
-      <c r="N60" s="15">
-        <f t="shared" si="3"/>
+      <c r="O60" s="15">
+        <f t="shared" si="4"/>
         <v>1.238660980232873</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T60" s="15">
+        <f t="shared" si="7"/>
+        <v>0.98119170306047609</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>39</v>
       </c>
@@ -3929,7 +4325,7 @@
         <v>98.841899999999995</v>
       </c>
       <c r="H61" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>98.406499999999994</v>
       </c>
       <c r="I61">
@@ -3942,19 +4338,24 @@
         <v>100.785</v>
       </c>
       <c r="L61" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101.62466666666667</v>
       </c>
-      <c r="M61" s="15">
-        <f t="shared" si="2"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15">
+        <f t="shared" si="3"/>
         <v>2.2524835195019226</v>
       </c>
-      <c r="N61" s="15">
-        <f t="shared" si="3"/>
+      <c r="O61" s="15">
+        <f t="shared" si="4"/>
         <v>2.3261460050051883</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T61" s="15">
+        <f t="shared" si="7"/>
+        <v>1.0715470677385159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>31</v>
       </c>
@@ -3971,7 +4372,7 @@
         <v>147.613</v>
       </c>
       <c r="H62" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>147.95066666666668</v>
       </c>
       <c r="I62">
@@ -3984,19 +4385,24 @@
         <v>148.38800000000001</v>
       </c>
       <c r="L62" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>148.29400000000001</v>
       </c>
-      <c r="M62" s="15">
-        <f t="shared" si="2"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15">
+        <f t="shared" si="3"/>
         <v>2.9891137083766868</v>
       </c>
-      <c r="N62" s="15">
-        <f t="shared" si="3"/>
+      <c r="O62" s="15">
+        <f t="shared" si="4"/>
         <v>2.9960502257735397</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T62" s="15">
+        <f t="shared" si="7"/>
+        <v>1.161726496217512</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>41</v>
       </c>
@@ -4013,7 +4419,7 @@
         <v>193.60499999999999</v>
       </c>
       <c r="H63" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194.19399999999999</v>
       </c>
       <c r="I63">
@@ -4026,19 +4432,24 @@
         <v>199.452</v>
       </c>
       <c r="L63" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198.34966666666665</v>
       </c>
-      <c r="M63" s="15">
-        <f t="shared" si="2"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15">
+        <f t="shared" si="3"/>
         <v>4.1770235099266522</v>
       </c>
-      <c r="N63" s="15">
-        <f t="shared" si="3"/>
+      <c r="O63" s="15">
+        <f t="shared" si="4"/>
         <v>4.2664099861621958</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T63" s="15">
+        <f t="shared" si="7"/>
+        <v>1.2563769073714746</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>46</v>
       </c>
@@ -4055,7 +4466,7 @@
         <v>241.297</v>
       </c>
       <c r="H64" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>241.17333333333332</v>
       </c>
       <c r="I64">
@@ -4068,19 +4479,24 @@
         <v>272.08499999999998</v>
       </c>
       <c r="L64" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>269.47899999999998</v>
       </c>
-      <c r="M64" s="15">
-        <f t="shared" si="2"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15">
+        <f t="shared" si="3"/>
         <v>4.409712191191546</v>
       </c>
-      <c r="N64" s="15">
-        <f t="shared" si="3"/>
+      <c r="O64" s="15">
+        <f t="shared" si="4"/>
         <v>4.9272646156434101</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T64" s="15">
+        <f t="shared" si="7"/>
+        <v>1.3148352953039564</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>32</v>
       </c>
@@ -4097,7 +4513,7 @@
         <v>191.51499999999999</v>
       </c>
       <c r="H65" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>187.16133333333332</v>
       </c>
       <c r="I65">
@@ -4110,19 +4526,24 @@
         <v>138.80099999999999</v>
       </c>
       <c r="L65" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>139.71133333333333</v>
       </c>
-      <c r="M65" s="15">
-        <f t="shared" si="2"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15">
+        <f t="shared" si="3"/>
         <v>3.9978411754486389</v>
       </c>
-      <c r="N65" s="15">
-        <f t="shared" si="3"/>
+      <c r="O65" s="15">
+        <f t="shared" si="4"/>
         <v>2.9842901369059311</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T65" s="20">
+        <f t="shared" si="7"/>
+        <v>0.81507266217969032</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>34</v>
       </c>
@@ -4139,7 +4560,7 @@
         <v>175.18600000000001</v>
       </c>
       <c r="H66" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>169.24433333333334</v>
       </c>
       <c r="I66">
@@ -4152,19 +4573,27 @@
         <v>129.46</v>
       </c>
       <c r="L66" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>129.28366666666668</v>
       </c>
-      <c r="M66" s="15">
-        <f t="shared" si="2"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15">
+        <f t="shared" si="3"/>
         <v>3.403195860395595</v>
       </c>
-      <c r="N66" s="15">
-        <f t="shared" si="3"/>
+      <c r="O66" s="15">
+        <f t="shared" si="4"/>
         <v>2.5996595014511406</v>
       </c>
+      <c r="T66" s="20">
+        <f t="shared" si="7"/>
+        <v>0.72589541218812403</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="T19:U35">
+    <sortCondition ref="T19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added perf measurements of master-candidate on 24/6/2015 (709637105b)
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="136">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>TX56Mbps</t>
+  </si>
+  <si>
+    <t>master-candidate, 24/6/2015</t>
+  </si>
+  <si>
+    <t>ratio</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,6 +582,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +886,7 @@
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>48</v>
       </c>
@@ -913,8 +923,16 @@
       <c r="L1" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -949,7 +967,7 @@
         <v>0.56783910298279994</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
@@ -984,7 +1002,7 @@
         <v>0.71543710570361785</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1037,7 @@
         <v>0.37316944295181803</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>0.90756843800322062</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1107,7 @@
         <v>3.3603208292201381</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1124,7 +1142,7 @@
         <v>3.2087631763879125</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1177,7 @@
         <v>0.71934874522640468</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1212,7 @@
         <v>1.1732229522558038</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1247,7 @@
         <v>3.9601844532279316</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>1</v>
       </c>
@@ -1264,7 +1282,7 @@
         <v>0.71771923822556727</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
@@ -1299,7 +1317,7 @@
         <v>1.1352241297091081</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
@@ -1334,7 +1352,7 @@
         <v>0.79322880371660853</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1387,7 @@
         <v>0.59702129531854975</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +1422,7 @@
         <v>0.46812395309882748</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -1999,7 +2017,7 @@
         <v>0.7924707070707071</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>47</v>
       </c>
@@ -2033,8 +2051,21 @@
         <f t="shared" si="1"/>
         <v>0.84195116772823775</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>137.38300000000001</v>
+      </c>
+      <c r="N33">
+        <v>136.977</v>
+      </c>
+      <c r="O33">
+        <v>136.78800000000001</v>
+      </c>
+      <c r="P33">
+        <f>$O33/$G33</f>
+        <v>1.0585176357698916</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
@@ -2068,8 +2099,21 @@
         <f t="shared" si="1"/>
         <v>0.86729078014184402</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>123.684</v>
+      </c>
+      <c r="N34">
+        <v>123.45399999999999</v>
+      </c>
+      <c r="O34">
+        <v>122.077</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ref="P34:P49" si="4">$O34/$G34</f>
+        <v>0.96848076160253871</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>42</v>
       </c>
@@ -2100,11 +2144,24 @@
         <v>1.1684713296058611</v>
       </c>
       <c r="J35" s="24">
-        <f>$H35/$C35</f>
+        <f t="shared" ref="J35:J42" si="5">$H35/$C35</f>
         <v>0.8969354354354353</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>100.416</v>
+      </c>
+      <c r="N35">
+        <v>98.441400000000002</v>
+      </c>
+      <c r="O35">
+        <v>99.717799999999997</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>0.99408639132298537</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>44</v>
       </c>
@@ -2135,11 +2192,24 @@
         <v>1.2779058830236003</v>
       </c>
       <c r="J36" s="24">
-        <f>$H36/$C36</f>
+        <f t="shared" si="5"/>
         <v>0.90573838383838379</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>89.561999999999998</v>
+      </c>
+      <c r="N36">
+        <v>89.119100000000003</v>
+      </c>
+      <c r="O36">
+        <v>88.350899999999996</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>0.9709572980956902</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>43</v>
       </c>
@@ -2170,11 +2240,24 @@
         <v>1.2077970807623624</v>
       </c>
       <c r="J37" s="24">
-        <f>$H37/$C37</f>
+        <f t="shared" si="5"/>
         <v>0.96878454106280187</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>65.986099999999993</v>
+      </c>
+      <c r="N37">
+        <v>65.811999999999998</v>
+      </c>
+      <c r="O37">
+        <v>65.389600000000002</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>0.95639938804105862</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>40</v>
       </c>
@@ -2205,11 +2288,24 @@
         <v>1.3473716416862755</v>
       </c>
       <c r="J38" s="24">
-        <f>$H38/$C38</f>
+        <f t="shared" si="5"/>
         <v>0.98105722222222236</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>56.328400000000002</v>
+      </c>
+      <c r="N38">
+        <v>55.880800000000001</v>
+      </c>
+      <c r="O38">
+        <v>56.274900000000002</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>0.95093327655605231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>33</v>
       </c>
@@ -2240,11 +2336,24 @@
         <v>1.5903185904784889</v>
       </c>
       <c r="J39" s="24">
-        <f>$H39/$C39</f>
+        <f t="shared" si="5"/>
         <v>1.1459282608695651</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>51.140500000000003</v>
+      </c>
+      <c r="N39">
+        <v>50.722900000000003</v>
+      </c>
+      <c r="O39">
+        <v>50.746099999999998</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>0.96380011433542068</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>37</v>
       </c>
@@ -2275,11 +2384,24 @@
         <v>1.7710518826052504</v>
       </c>
       <c r="J40" s="24">
-        <f>$H40/$C40</f>
+        <f t="shared" si="5"/>
         <v>1.2399370370370371</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>53.203000000000003</v>
+      </c>
+      <c r="N40">
+        <v>53.332099999999997</v>
+      </c>
+      <c r="O40">
+        <v>53.044800000000002</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>0.94750097795973487</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>35</v>
       </c>
@@ -2310,11 +2432,11 @@
         <v>1.0520976755487164</v>
       </c>
       <c r="J41" s="24">
-        <f>$H41/$C41</f>
+        <f t="shared" si="5"/>
         <v>0.89897923875432528</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>38</v>
       </c>
@@ -2345,11 +2467,24 @@
         <v>1.5623359015293492</v>
       </c>
       <c r="J42" s="24">
-        <f>$H42/$C42</f>
+        <f t="shared" si="5"/>
         <v>1.0420635802469136</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>57.195999999999998</v>
+      </c>
+      <c r="N42">
+        <v>58.373399999999997</v>
+      </c>
+      <c r="O42">
+        <v>57.666600000000003</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>1.0244391189339663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>45</v>
       </c>
@@ -2380,11 +2515,24 @@
         <v>1.6966693607625518</v>
       </c>
       <c r="J43" s="24">
-        <f t="shared" ref="J43:J66" si="4">$H43/$C43</f>
+        <f t="shared" ref="J43:J66" si="6">$H43/$C43</f>
         <v>1.0169064935064935</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>75.6023</v>
+      </c>
+      <c r="N43">
+        <v>75.1006</v>
+      </c>
+      <c r="O43">
+        <v>75.275700000000001</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>0.95629113665149401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>39</v>
       </c>
@@ -2415,11 +2563,24 @@
         <v>2.3009066917509338</v>
       </c>
       <c r="J44" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0483095238095237</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>97.427800000000005</v>
+      </c>
+      <c r="N44">
+        <v>97.807500000000005</v>
+      </c>
+      <c r="O44">
+        <v>94.270899999999997</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="4"/>
+        <v>0.91738013448681899</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>31</v>
       </c>
@@ -2450,11 +2611,24 @@
         <v>2.4323779287145708</v>
       </c>
       <c r="J45" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.98311922141119212</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>118.88200000000001</v>
+      </c>
+      <c r="N45">
+        <v>115.252</v>
+      </c>
+      <c r="O45">
+        <v>117.265</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>0.8689900995968699</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>41</v>
       </c>
@@ -2485,11 +2659,24 @@
         <v>3.3968780294689531</v>
       </c>
       <c r="J46" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2702988505747128</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>140.08199999999999</v>
+      </c>
+      <c r="N46">
+        <v>141.39400000000001</v>
+      </c>
+      <c r="O46">
+        <v>141.47399999999999</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="4"/>
+        <v>0.76928598228413891</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>46</v>
       </c>
@@ -2520,11 +2707,24 @@
         <v>3.3467427655828366</v>
       </c>
       <c r="J47" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0777749999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>162.01499999999999</v>
+      </c>
+      <c r="N47">
+        <v>161.41900000000001</v>
+      </c>
+      <c r="O47">
+        <v>159.86600000000001</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="4"/>
+        <v>0.73623468729851715</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>32</v>
       </c>
@@ -2555,12 +2755,25 @@
         <v>4.1643097013471717</v>
       </c>
       <c r="J48" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0025945165945167</v>
       </c>
       <c r="K48" s="18"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>183.38300000000001</v>
+      </c>
+      <c r="N48">
+        <v>181.37200000000001</v>
+      </c>
+      <c r="O48">
+        <v>182.89599999999999</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="4"/>
+        <v>0.78991785365685108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>34</v>
       </c>
@@ -2591,11 +2804,24 @@
         <v>3.4492312276283354</v>
       </c>
       <c r="J49" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.79285026041666662</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>164.583</v>
+      </c>
+      <c r="N49">
+        <v>161.56800000000001</v>
+      </c>
+      <c r="O49">
+        <v>161.518</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="4"/>
+        <v>0.79346629986244843</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>47</v>
       </c>
@@ -2623,7 +2849,7 @@
         <v>1.1916277158768707</v>
       </c>
       <c r="J50" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0278228070175437</v>
       </c>
       <c r="K50" s="27">
@@ -2635,7 +2861,7 @@
         <v>1.2101910828025477</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>36</v>
       </c>
@@ -2663,19 +2889,19 @@
         <v>1.2163220073608654</v>
       </c>
       <c r="J51" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0494298245614033</v>
       </c>
       <c r="K51" s="27">
-        <f t="shared" ref="K51:K66" si="5">$H51/$H34</f>
+        <f t="shared" ref="K51:K66" si="7">$H51/$H34</f>
         <v>1.6305088534170697</v>
       </c>
       <c r="L51" s="27">
-        <f t="shared" ref="L51:L66" si="6">$C51/$C34</f>
+        <f t="shared" ref="L51:L66" si="8">$C51/$C34</f>
         <v>1.3475177304964538</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
@@ -2703,7 +2929,7 @@
         <v>1.3943471648478118</v>
       </c>
       <c r="J52" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0338247619047618</v>
       </c>
       <c r="K52" s="15">
@@ -2711,11 +2937,11 @@
         <v>1.8171920068166714</v>
       </c>
       <c r="L52" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.5765765765765767</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>44</v>
       </c>
@@ -2743,19 +2969,19 @@
         <v>1.2714024647392344</v>
       </c>
       <c r="J53" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.77522857142857138</v>
       </c>
       <c r="K53" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.5129683800593523</v>
       </c>
       <c r="L53" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.7676767676767677</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>43</v>
       </c>
@@ -2783,19 +3009,19 @@
         <v>1.4347198105342529</v>
       </c>
       <c r="J54" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1620860215053763</v>
       </c>
       <c r="K54" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.6167576883030883</v>
       </c>
       <c r="L54" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3478260869565217</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>40</v>
       </c>
@@ -2823,19 +3049,19 @@
         <v>1.4413653280101908</v>
       </c>
       <c r="J55" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1790388127853881</v>
       </c>
       <c r="K55" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.4621952621406724</v>
       </c>
       <c r="L55" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2166666666666666</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>33</v>
       </c>
@@ -2863,19 +3089,19 @@
         <v>1.8800057889282078</v>
       </c>
       <c r="J56" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5792196078431373</v>
       </c>
       <c r="K56" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.5279088341139804</v>
       </c>
       <c r="L56" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1086956521739131</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>37</v>
       </c>
@@ -2903,19 +3129,19 @@
         <v>2.163487203642644</v>
       </c>
       <c r="J57" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.6931366013071893</v>
       </c>
       <c r="K57" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.5475690223219218</v>
       </c>
       <c r="L57" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1333333333333333</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>35</v>
       </c>
@@ -2943,7 +3169,7 @@
       <c r="K58" s="15"/>
       <c r="L58" s="27"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>38</v>
       </c>
@@ -2971,19 +3197,19 @@
         <v>1.1101745758402708</v>
       </c>
       <c r="J59" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0276153333333333</v>
       </c>
       <c r="K59" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.91308793153186663</v>
       </c>
       <c r="L59" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.92592592592592593</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>45</v>
       </c>
@@ -3011,19 +3237,19 @@
         <v>1.2882683455185486</v>
       </c>
       <c r="J60" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0286648648648649</v>
       </c>
       <c r="K60" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.97215134262558467</v>
       </c>
       <c r="L60" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.96103896103896103</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>39</v>
       </c>
@@ -3051,19 +3277,19 @@
         <v>2.3835988524690226</v>
       </c>
       <c r="J61" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0413466666666666</v>
       </c>
       <c r="K61" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0136306265675545</v>
       </c>
       <c r="L61" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0204081632653061</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>31</v>
       </c>
@@ -3091,19 +3317,19 @@
         <v>3.1370231565194842</v>
       </c>
       <c r="J62" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.98899150743099773</v>
       </c>
       <c r="K62" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.1528305062094431</v>
       </c>
       <c r="L62" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1459854014598541</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>41</v>
       </c>
@@ -3131,19 +3357,19 @@
         <v>4.2959712632552538</v>
       </c>
       <c r="J63" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.97426341463414645</v>
       </c>
       <c r="K63" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.084317202938941</v>
       </c>
       <c r="L63" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.4137931034482758</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>46</v>
       </c>
@@ -3171,15 +3397,15 @@
         <v>5.3334466966774796</v>
       </c>
       <c r="J64" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99895091324200935</v>
       </c>
       <c r="K64" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.3532215289214666</v>
       </c>
       <c r="L64" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.46</v>
       </c>
     </row>
@@ -3211,15 +3437,15 @@
         <v>6.4401111310474857</v>
       </c>
       <c r="J65" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.75374416666666677</v>
       </c>
       <c r="K65" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.3018071439468739</v>
       </c>
       <c r="L65" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.7316017316017316</v>
       </c>
     </row>
@@ -3251,19 +3477,134 @@
         <v>5.2343541587071787</v>
       </c>
       <c r="J66" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.57846592592592605</v>
       </c>
       <c r="K66" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.282505267617986</v>
       </c>
       <c r="L66" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.7578125</v>
       </c>
     </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="F68" s="28">
+        <v>1614.74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="18">
+        <v>1876.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="18">
+        <v>2328.5700000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>182.77600000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="18">
+        <v>1869.31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="18">
+        <v>975.83699999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74">
+        <v>1571.86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75">
+        <v>1563.07</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76">
+        <v>1851.71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77">
+        <v>2359.25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78">
+        <v>2266.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79">
+        <v>1174.17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="18">
+        <v>1570.43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="18">
+        <v>1908.83</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added performance results for new-c-lib
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -16,7 +16,7 @@
     <sheet name="TX Optim" sheetId="3" r:id="rId2"/>
     <sheet name="Old" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,16 +430,16 @@
     <t>TX56Mbps</t>
   </si>
   <si>
-    <t>master-candidate, 24/6/2015</t>
-  </si>
-  <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>new-c-lib, 21/8/2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -537,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -583,9 +583,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,8 +865,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +882,8 @@
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -923,14 +923,14 @@
       <c r="L1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="16" t="s">
-        <v>135</v>
-      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -966,6 +966,13 @@
         <f t="shared" ref="J2:J34" si="1">$H2/$C2</f>
         <v>0.56783910298279994</v>
       </c>
+      <c r="M2">
+        <v>1539.4</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N32" si="2">$M2/$G2</f>
+        <v>0.89114011982980701</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -990,7 +997,7 @@
         <v>1847.69</v>
       </c>
       <c r="H3" s="24">
-        <f t="shared" ref="H3:H66" si="2">AVERAGE($E3, $F3, $G3)</f>
+        <f t="shared" ref="H3:H66" si="3">AVERAGE($E3, $F3, $G3)</f>
         <v>1852.2666666666667</v>
       </c>
       <c r="I3" s="15">
@@ -1001,6 +1008,13 @@
         <f t="shared" si="1"/>
         <v>0.71543710570361785</v>
       </c>
+      <c r="M3">
+        <v>1390.86</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="2"/>
+        <v>0.75275614415838144</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1025,7 +1039,7 @@
         <v>1382.34</v>
       </c>
       <c r="H4" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1388.9366666666667</v>
       </c>
       <c r="I4" s="15">
@@ -1036,6 +1050,13 @@
         <f t="shared" si="1"/>
         <v>0.37316944295181803</v>
       </c>
+      <c r="M4">
+        <v>1160.8800000000001</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>0.83979339381049534</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1060,7 +1081,7 @@
         <v>188.38399999999999</v>
       </c>
       <c r="H5" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>187.86666666666667</v>
       </c>
       <c r="I5" s="15">
@@ -1071,6 +1092,13 @@
         <f t="shared" si="1"/>
         <v>0.90756843800322062</v>
       </c>
+      <c r="M5">
+        <v>210.202</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>1.1158166298624088</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -1095,7 +1123,7 @@
         <v>6858.57</v>
       </c>
       <c r="H6" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6808.0099999999993</v>
       </c>
       <c r="I6" s="15">
@@ -1106,6 +1134,13 @@
         <f t="shared" si="1"/>
         <v>3.3603208292201381</v>
       </c>
+      <c r="M6">
+        <v>5207.76</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0.75930696923702756</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -1130,7 +1165,7 @@
         <v>4504.71</v>
       </c>
       <c r="H7" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4566.07</v>
       </c>
       <c r="I7" s="15">
@@ -1141,6 +1176,13 @@
         <f t="shared" si="1"/>
         <v>3.2087631763879125</v>
       </c>
+      <c r="M7">
+        <v>2983.24</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0.66224906819750873</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -1165,7 +1207,7 @@
         <v>3707.12</v>
       </c>
       <c r="H8" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3516.1766666666663</v>
       </c>
       <c r="I8" s="15">
@@ -1176,6 +1218,13 @@
         <f t="shared" si="1"/>
         <v>0.71934874522640468</v>
       </c>
+      <c r="M8">
+        <v>6841.68</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>1.8455512635145344</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -1200,7 +1249,7 @@
         <v>4465.0200000000004</v>
       </c>
       <c r="H9" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4464.1133333333337</v>
       </c>
       <c r="I9" s="15">
@@ -1211,6 +1260,13 @@
         <f t="shared" si="1"/>
         <v>1.1732229522558038</v>
       </c>
+      <c r="M9">
+        <v>6274.98</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>1.4053643656691346</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1235,7 +1291,7 @@
         <v>2980.07</v>
       </c>
       <c r="H10" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3005.78</v>
       </c>
       <c r="I10" s="15">
@@ -1246,6 +1302,13 @@
         <f t="shared" si="1"/>
         <v>3.9601844532279316</v>
       </c>
+      <c r="M10">
+        <v>5273.54</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>1.7696027274527106</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1270,7 +1333,7 @@
         <v>2124.46</v>
       </c>
       <c r="H11" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2097.893333333333</v>
       </c>
       <c r="I11" s="15">
@@ -1281,6 +1344,13 @@
         <f t="shared" si="1"/>
         <v>0.71771923822556727</v>
       </c>
+      <c r="M11">
+        <v>2092.4899999999998</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>0.98495147002061689</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -1305,7 +1375,7 @@
         <v>3125.9</v>
       </c>
       <c r="H12" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3174.0866666666666</v>
       </c>
       <c r="I12" s="15">
@@ -1316,6 +1386,13 @@
         <f t="shared" si="1"/>
         <v>1.1352241297091081</v>
       </c>
+      <c r="M12">
+        <v>2983.24</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>0.95436194376019701</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1340,7 +1417,7 @@
         <v>2255.9499999999998</v>
       </c>
       <c r="H13" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2276.5666666666666</v>
       </c>
       <c r="I13" s="15">
@@ -1351,6 +1428,13 @@
         <f t="shared" si="1"/>
         <v>0.79322880371660853</v>
       </c>
+      <c r="M13">
+        <v>2093.16</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>0.92783971275959132</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1375,7 +1459,7 @@
         <v>2249.1799999999998</v>
       </c>
       <c r="H14" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2261.5166666666664</v>
       </c>
       <c r="I14" s="15">
@@ -1386,6 +1470,13 @@
         <f t="shared" si="1"/>
         <v>0.59702129531854975</v>
       </c>
+      <c r="M14">
+        <v>2095.7199999999998</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>0.93177068976249122</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1410,7 +1501,7 @@
         <v>1816.38</v>
       </c>
       <c r="H15" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1769.9766666666667</v>
       </c>
       <c r="I15" s="15">
@@ -1421,6 +1512,13 @@
         <f t="shared" si="1"/>
         <v>0.46812395309882748</v>
       </c>
+      <c r="M15">
+        <v>1405.36</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.7737147513185566</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1445,7 +1543,7 @@
         <v>145.298</v>
       </c>
       <c r="H16" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145.25666666666666</v>
       </c>
       <c r="I16" s="15">
@@ -1456,8 +1554,15 @@
         <f t="shared" si="1"/>
         <v>0.75262521588946452</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>188.94499999999999</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>1.3003964266541865</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1585,7 @@
         <v>1186.83</v>
       </c>
       <c r="H17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1189.9633333333334</v>
       </c>
       <c r="I17" s="15">
@@ -1491,8 +1596,15 @@
         <f t="shared" si="1"/>
         <v>0.70831150793650799</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>1074.69</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>0.90551300523242595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>28</v>
       </c>
@@ -1515,7 +1627,7 @@
         <v>2763.88</v>
       </c>
       <c r="H18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2332.1533333333332</v>
       </c>
       <c r="I18" s="15">
@@ -1526,8 +1638,15 @@
         <f t="shared" si="1"/>
         <v>0.48840907504363001</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>7647.01</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>2.7667662850774999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>22</v>
       </c>
@@ -1550,7 +1669,7 @@
         <v>1803.2</v>
       </c>
       <c r="H19" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1683.6899999999998</v>
       </c>
       <c r="I19" s="15">
@@ -1561,8 +1680,15 @@
         <f t="shared" si="1"/>
         <v>0.57209989806320072</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1934.91</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>1.0730423691215616</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
@@ -1585,7 +1711,7 @@
         <v>1813.53</v>
       </c>
       <c r="H20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1687.3133333333333</v>
       </c>
       <c r="I20" s="15">
@@ -1596,8 +1722,15 @@
         <f t="shared" si="1"/>
         <v>0.50945450885668275</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>2784.89</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>1.5356183796242686</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1753,7 @@
         <v>1772.11</v>
       </c>
       <c r="H21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1790.4899999999998</v>
       </c>
       <c r="I21" s="15">
@@ -1631,8 +1764,15 @@
         <f t="shared" si="1"/>
         <v>0.53209212481426438</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>2895.61</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>1.633989989334748</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>15</v>
       </c>
@@ -1655,7 +1795,7 @@
         <v>2542.0700000000002</v>
       </c>
       <c r="H22" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1942.28</v>
       </c>
       <c r="I22" s="15">
@@ -1666,8 +1806,15 @@
         <f t="shared" si="1"/>
         <v>0.6223261775072092</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>2426.12</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>0.95438756603870067</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -1690,7 +1837,7 @@
         <v>1419.67</v>
       </c>
       <c r="H23" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1486.1966666666667</v>
       </c>
       <c r="I23" s="15">
@@ -1701,8 +1848,15 @@
         <f t="shared" si="1"/>
         <v>1.7161624326404927</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>1877.48</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>1.3224763501377079</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>23</v>
       </c>
@@ -1725,7 +1879,7 @@
         <v>587.75099999999998</v>
       </c>
       <c r="H24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>586.67766666666671</v>
       </c>
       <c r="I24" s="15">
@@ -1736,8 +1890,15 @@
         <f t="shared" si="1"/>
         <v>0.92682095839915757</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>296.27499999999998</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>0.50408251113141445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
@@ -1760,7 +1921,7 @@
         <v>460.65300000000002</v>
       </c>
       <c r="H25" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>447.42533333333336</v>
       </c>
       <c r="I25" s="15">
@@ -1771,8 +1932,15 @@
         <f t="shared" si="1"/>
         <v>0.8571366538952746</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>183.07900000000001</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>0.39743364311097507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>25</v>
       </c>
@@ -1795,7 +1963,7 @@
         <v>1088.29</v>
       </c>
       <c r="H26" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>936.36700000000008</v>
       </c>
       <c r="I26" s="15">
@@ -1806,8 +1974,15 @@
         <f t="shared" si="1"/>
         <v>1.2304428383705652</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>651.85599999999999</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>0.59897270029128269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>18</v>
       </c>
@@ -1830,7 +2005,7 @@
         <v>3367.8</v>
       </c>
       <c r="H27" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2974.6033333333339</v>
       </c>
       <c r="I27" s="15">
@@ -1841,8 +2016,15 @@
         <f t="shared" si="1"/>
         <v>2.6115920398009957</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>5048.72</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>1.4991151493556625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>24</v>
       </c>
@@ -1865,7 +2047,7 @@
         <v>428.22</v>
       </c>
       <c r="H28" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>443.60399999999998</v>
       </c>
       <c r="I28" s="15">
@@ -1876,8 +2058,15 @@
         <f t="shared" si="1"/>
         <v>0.95398709677419347</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>495.09399999999999</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>1.1561673905936201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>16</v>
       </c>
@@ -1900,7 +2089,7 @@
         <v>223.45599999999999</v>
       </c>
       <c r="H29" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>223.14566666666667</v>
       </c>
       <c r="I29" s="15">
@@ -1911,8 +2100,15 @@
         <f t="shared" si="1"/>
         <v>0.61303754578754577</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>315.16399999999999</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>1.4104074180151798</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>26</v>
       </c>
@@ -1935,7 +2131,7 @@
         <v>326.02600000000001</v>
       </c>
       <c r="H30" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>326.78966666666673</v>
       </c>
       <c r="I30" s="15">
@@ -1946,8 +2142,15 @@
         <f t="shared" si="1"/>
         <v>0.7512406130268201</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>311.40899999999999</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>0.95516615239275393</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
@@ -1970,7 +2173,7 @@
         <v>1222.8699999999999</v>
       </c>
       <c r="H31" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1362.6033333333332</v>
       </c>
       <c r="I31" s="15">
@@ -1981,8 +2184,15 @@
         <f t="shared" si="1"/>
         <v>2.1158436853002067</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>397.548</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>0.32509424550442811</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>30</v>
       </c>
@@ -2005,7 +2215,7 @@
         <v>130.44399999999999</v>
       </c>
       <c r="H32" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130.75766666666667</v>
       </c>
       <c r="I32" s="15">
@@ -2016,8 +2226,15 @@
         <f t="shared" si="1"/>
         <v>0.7924707070707071</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>115.545</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>0.88578240471006719</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>47</v>
       </c>
@@ -2040,7 +2257,7 @@
         <v>129.226</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132.18633333333332</v>
       </c>
       <c r="I33" s="15">
@@ -2052,20 +2269,14 @@
         <v>0.84195116772823775</v>
       </c>
       <c r="M33">
-        <v>137.38300000000001</v>
+        <v>144.15299999999999</v>
       </c>
       <c r="N33">
-        <v>136.977</v>
-      </c>
-      <c r="O33">
-        <v>136.78800000000001</v>
-      </c>
-      <c r="P33">
-        <f>$O33/$G33</f>
-        <v>1.0585176357698916</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M33/$G33</f>
+        <v>1.1155108105180072</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
@@ -2088,11 +2299,11 @@
         <v>126.05</v>
       </c>
       <c r="H34" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122.28800000000001</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" ref="I34:I66" si="3">$H34/$D34</f>
+        <f t="shared" ref="I34:I66" si="4">$H34/$D34</f>
         <v>1.1471992645196396</v>
       </c>
       <c r="J34" s="24">
@@ -2100,20 +2311,14 @@
         <v>0.86729078014184402</v>
       </c>
       <c r="M34">
-        <v>123.684</v>
+        <v>128.56</v>
       </c>
       <c r="N34">
-        <v>123.45399999999999</v>
-      </c>
-      <c r="O34">
-        <v>122.077</v>
-      </c>
-      <c r="P34">
-        <f t="shared" ref="P34:P49" si="4">$O34/$G34</f>
-        <v>0.96848076160253871</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M34/$G34</f>
+        <v>1.0199127330424436</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>42</v>
       </c>
@@ -2136,11 +2341,11 @@
         <v>100.31100000000001</v>
       </c>
       <c r="H35" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99.559833333333316</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1684713296058611</v>
       </c>
       <c r="J35" s="24">
@@ -2148,20 +2353,14 @@
         <v>0.8969354354354353</v>
       </c>
       <c r="M35">
-        <v>100.416</v>
+        <v>103.568</v>
       </c>
       <c r="N35">
-        <v>98.441400000000002</v>
-      </c>
-      <c r="O35">
-        <v>99.717799999999997</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="4"/>
-        <v>0.99408639132298537</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M35/$G35</f>
+        <v>1.0324690213436212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>44</v>
       </c>
@@ -2184,11 +2383,11 @@
         <v>90.993600000000001</v>
       </c>
       <c r="H36" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89.668099999999995</v>
       </c>
       <c r="I36" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2779058830236003</v>
       </c>
       <c r="J36" s="24">
@@ -2196,20 +2395,14 @@
         <v>0.90573838383838379</v>
       </c>
       <c r="M36">
-        <v>89.561999999999998</v>
+        <v>86.337100000000007</v>
       </c>
       <c r="N36">
-        <v>89.119100000000003</v>
-      </c>
-      <c r="O36">
-        <v>88.350899999999996</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="4"/>
-        <v>0.9709572980956902</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M36/$G36</f>
+        <v>0.94882607128413432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>43</v>
       </c>
@@ -2232,11 +2425,11 @@
         <v>68.370599999999996</v>
       </c>
       <c r="H37" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66.846133333333327</v>
       </c>
       <c r="I37" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2077970807623624</v>
       </c>
       <c r="J37" s="24">
@@ -2244,20 +2437,14 @@
         <v>0.96878454106280187</v>
       </c>
       <c r="M37">
-        <v>65.986099999999993</v>
+        <v>68.238</v>
       </c>
       <c r="N37">
-        <v>65.811999999999998</v>
-      </c>
-      <c r="O37">
-        <v>65.389600000000002</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="4"/>
-        <v>0.95639938804105862</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M37/$G37</f>
+        <v>0.99806056989407732</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>40</v>
       </c>
@@ -2280,11 +2467,11 @@
         <v>59.178600000000003</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58.86343333333334</v>
       </c>
       <c r="I38" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3473716416862755</v>
       </c>
       <c r="J38" s="24">
@@ -2292,20 +2479,14 @@
         <v>0.98105722222222236</v>
       </c>
       <c r="M38">
-        <v>56.328400000000002</v>
+        <v>57.339500000000001</v>
       </c>
       <c r="N38">
-        <v>55.880800000000001</v>
-      </c>
-      <c r="O38">
-        <v>56.274900000000002</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="4"/>
-        <v>0.95093327655605231</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M38/$G38</f>
+        <v>0.96892288766547363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>33</v>
       </c>
@@ -2332,7 +2513,7 @@
         <v>52.712699999999991</v>
       </c>
       <c r="I39" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5903185904784889</v>
       </c>
       <c r="J39" s="24">
@@ -2340,20 +2521,14 @@
         <v>1.1459282608695651</v>
       </c>
       <c r="M39">
-        <v>51.140500000000003</v>
+        <v>53.083500000000001</v>
       </c>
       <c r="N39">
-        <v>50.722900000000003</v>
-      </c>
-      <c r="O39">
-        <v>50.746099999999998</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="4"/>
-        <v>0.96380011433542068</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M39/$G39</f>
+        <v>1.008193405391238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>37</v>
       </c>
@@ -2376,11 +2551,11 @@
         <v>55.983899999999998</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55.797166666666669</v>
       </c>
       <c r="I40" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7710518826052504</v>
       </c>
       <c r="J40" s="24">
@@ -2388,20 +2563,14 @@
         <v>1.2399370370370371</v>
       </c>
       <c r="M40">
-        <v>53.203000000000003</v>
+        <v>55.146500000000003</v>
       </c>
       <c r="N40">
-        <v>53.332099999999997</v>
-      </c>
-      <c r="O40">
-        <v>53.044800000000002</v>
-      </c>
-      <c r="P40">
-        <f t="shared" si="4"/>
-        <v>0.94750097795973487</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M40/$G40</f>
+        <v>0.9850421281832813</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>35</v>
       </c>
@@ -2424,19 +2593,26 @@
         <v>259.875</v>
       </c>
       <c r="H41" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>259.80500000000001</v>
       </c>
       <c r="I41" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0520976755487164</v>
       </c>
       <c r="J41" s="24">
         <f t="shared" si="5"/>
         <v>0.89897923875432528</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>245.54300000000001</v>
+      </c>
+      <c r="N41">
+        <f>$M41/$G41</f>
+        <v>0.94485040885040883</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>38</v>
       </c>
@@ -2459,11 +2635,11 @@
         <v>56.290900000000001</v>
       </c>
       <c r="H42" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56.271433333333334</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5623359015293492</v>
       </c>
       <c r="J42" s="24">
@@ -2471,20 +2647,14 @@
         <v>1.0420635802469136</v>
       </c>
       <c r="M42">
-        <v>57.195999999999998</v>
+        <v>65.837800000000001</v>
       </c>
       <c r="N42">
-        <v>58.373399999999997</v>
-      </c>
-      <c r="O42">
-        <v>57.666600000000003</v>
-      </c>
-      <c r="P42">
-        <f t="shared" si="4"/>
-        <v>1.0244391189339663</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M42/$G42</f>
+        <v>1.1695993490955021</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>45</v>
       </c>
@@ -2507,11 +2677,11 @@
         <v>78.716300000000004</v>
       </c>
       <c r="H43" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78.3018</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6966693607625518</v>
       </c>
       <c r="J43" s="24">
@@ -2519,20 +2689,14 @@
         <v>1.0169064935064935</v>
       </c>
       <c r="M43">
-        <v>75.6023</v>
+        <v>90.422499999999999</v>
       </c>
       <c r="N43">
-        <v>75.1006</v>
-      </c>
-      <c r="O43">
-        <v>75.275700000000001</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="4"/>
-        <v>0.95629113665149401</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M43/$G43</f>
+        <v>1.1487137987938965</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>39</v>
       </c>
@@ -2555,11 +2719,11 @@
         <v>102.761</v>
       </c>
       <c r="H44" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102.73433333333332</v>
       </c>
       <c r="I44" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3009066917509338</v>
       </c>
       <c r="J44" s="24">
@@ -2567,20 +2731,14 @@
         <v>1.0483095238095237</v>
       </c>
       <c r="M44">
-        <v>97.427800000000005</v>
+        <v>123.629</v>
       </c>
       <c r="N44">
-        <v>97.807500000000005</v>
-      </c>
-      <c r="O44">
-        <v>94.270899999999997</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="4"/>
-        <v>0.91738013448681899</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M44/$G44</f>
+        <v>1.2030731503196739</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>31</v>
       </c>
@@ -2603,11 +2761,11 @@
         <v>134.94399999999999</v>
       </c>
       <c r="H45" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>134.68733333333333</v>
       </c>
       <c r="I45" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4323779287145708</v>
       </c>
       <c r="J45" s="24">
@@ -2615,20 +2773,14 @@
         <v>0.98311922141119212</v>
       </c>
       <c r="M45">
-        <v>118.88200000000001</v>
+        <v>157.97</v>
       </c>
       <c r="N45">
-        <v>115.252</v>
-      </c>
-      <c r="O45">
-        <v>117.265</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="4"/>
-        <v>0.8689900995968699</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M45/$G45</f>
+        <v>1.1706337443680341</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>41</v>
       </c>
@@ -2651,11 +2803,11 @@
         <v>183.90299999999999</v>
       </c>
       <c r="H46" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>184.19333333333336</v>
       </c>
       <c r="I46" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3968780294689531</v>
       </c>
       <c r="J46" s="24">
@@ -2663,20 +2815,14 @@
         <v>1.2702988505747128</v>
       </c>
       <c r="M46">
-        <v>140.08199999999999</v>
+        <v>208.244</v>
       </c>
       <c r="N46">
-        <v>141.39400000000001</v>
-      </c>
-      <c r="O46">
-        <v>141.47399999999999</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="4"/>
-        <v>0.76928598228413891</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M46/$G46</f>
+        <v>1.1323578190676606</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>46</v>
       </c>
@@ -2699,11 +2845,11 @@
         <v>217.14</v>
       </c>
       <c r="H47" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>215.55499999999998</v>
       </c>
       <c r="I47" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3467427655828366</v>
       </c>
       <c r="J47" s="24">
@@ -2711,20 +2857,14 @@
         <v>1.0777749999999999</v>
       </c>
       <c r="M47">
-        <v>162.01499999999999</v>
+        <v>240.614</v>
       </c>
       <c r="N47">
-        <v>161.41900000000001</v>
-      </c>
-      <c r="O47">
-        <v>159.86600000000001</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="4"/>
-        <v>0.73623468729851715</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M47/$G47</f>
+        <v>1.1081053698074976</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>32</v>
       </c>
@@ -2747,11 +2887,11 @@
         <v>231.53800000000001</v>
       </c>
       <c r="H48" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>231.59933333333333</v>
       </c>
       <c r="I48" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.1643097013471717</v>
       </c>
       <c r="J48" s="24">
@@ -2760,20 +2900,14 @@
       </c>
       <c r="K48" s="18"/>
       <c r="M48">
-        <v>183.38300000000001</v>
+        <v>233.05799999999999</v>
       </c>
       <c r="N48">
-        <v>181.37200000000001</v>
-      </c>
-      <c r="O48">
-        <v>182.89599999999999</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="4"/>
-        <v>0.78991785365685108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M48/$G48</f>
+        <v>1.0065647971391305</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>34</v>
       </c>
@@ -2796,11 +2930,11 @@
         <v>203.56</v>
       </c>
       <c r="H49" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>202.96966666666665</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4492312276283354</v>
       </c>
       <c r="J49" s="24">
@@ -2808,20 +2942,14 @@
         <v>0.79285026041666662</v>
       </c>
       <c r="M49">
-        <v>164.583</v>
+        <v>226.64099999999999</v>
       </c>
       <c r="N49">
-        <v>161.56800000000001</v>
-      </c>
-      <c r="O49">
-        <v>161.518</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="4"/>
-        <v>0.79346629986244843</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+        <f>$M49/$G49</f>
+        <v>1.1133867164472391</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>47</v>
       </c>
@@ -2841,11 +2969,11 @@
         <v>208.631</v>
       </c>
       <c r="H50" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>195.28633333333332</v>
       </c>
       <c r="I50" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1916277158768707</v>
       </c>
       <c r="J50" s="24">
@@ -2861,7 +2989,7 @@
         <v>1.2101910828025477</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>36</v>
       </c>
@@ -2881,11 +3009,11 @@
         <v>206.92400000000001</v>
       </c>
       <c r="H51" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199.39166666666665</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2163220073608654</v>
       </c>
       <c r="J51" s="24">
@@ -2901,7 +3029,7 @@
         <v>1.3475177304964538</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
@@ -2921,11 +3049,11 @@
         <v>184.93899999999999</v>
       </c>
       <c r="H52" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180.9193333333333</v>
       </c>
       <c r="I52" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3943471648478118</v>
       </c>
       <c r="J52" s="24">
@@ -2941,7 +3069,7 @@
         <v>1.5765765765765767</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>44</v>
       </c>
@@ -2961,11 +3089,11 @@
         <v>108.59099999999999</v>
       </c>
       <c r="H53" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>135.66499999999999</v>
       </c>
       <c r="I53" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2714024647392344</v>
       </c>
       <c r="J53" s="24">
@@ -2981,7 +3109,7 @@
         <v>1.7676767676767677</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>43</v>
       </c>
@@ -3001,11 +3129,11 @@
         <v>108.88500000000001</v>
       </c>
       <c r="H54" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108.074</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4347198105342529</v>
       </c>
       <c r="J54" s="24">
@@ -3021,7 +3149,7 @@
         <v>1.3478260869565217</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>40</v>
       </c>
@@ -3041,11 +3169,11 @@
         <v>83.654700000000005</v>
       </c>
       <c r="H55" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86.069833333333335</v>
       </c>
       <c r="I55" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4413653280101908</v>
       </c>
       <c r="J55" s="24">
@@ -3061,7 +3189,7 @@
         <v>1.2166666666666666</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>33</v>
       </c>
@@ -3081,11 +3209,11 @@
         <v>81.540099999999995</v>
       </c>
       <c r="H56" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80.540199999999999</v>
       </c>
       <c r="I56" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8800057889282078</v>
       </c>
       <c r="J56" s="24">
@@ -3101,7 +3229,7 @@
         <v>1.1086956521739131</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>37</v>
       </c>
@@ -3121,11 +3249,11 @@
         <v>88.773600000000002</v>
       </c>
       <c r="H57" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86.34996666666666</v>
       </c>
       <c r="I57" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.163487203642644</v>
       </c>
       <c r="J57" s="24">
@@ -3141,7 +3269,7 @@
         <v>1.1333333333333333</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>35</v>
       </c>
@@ -3158,18 +3286,18 @@
         <v>34.787199999999999</v>
       </c>
       <c r="H58" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34.685566666666666</v>
       </c>
       <c r="I58" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15912927254848885</v>
       </c>
       <c r="J58" s="24"/>
       <c r="K58" s="15"/>
       <c r="L58" s="27"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>38</v>
       </c>
@@ -3189,11 +3317,11 @@
         <v>52.1584</v>
       </c>
       <c r="H59" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51.380766666666666</v>
       </c>
       <c r="I59" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1101745758402708</v>
       </c>
       <c r="J59" s="24">
@@ -3209,7 +3337,7 @@
         <v>0.92592592592592593</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>45</v>
       </c>
@@ -3229,11 +3357,11 @@
         <v>74.287800000000004</v>
       </c>
       <c r="H60" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76.121200000000002</v>
       </c>
       <c r="I60" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2882683455185486</v>
       </c>
       <c r="J60" s="24">
@@ -3249,7 +3377,7 @@
         <v>0.96103896103896103</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>39</v>
       </c>
@@ -3269,11 +3397,11 @@
         <v>104.67700000000001</v>
       </c>
       <c r="H61" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104.13466666666666</v>
       </c>
       <c r="I61" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3835988524690226</v>
       </c>
       <c r="J61" s="24">
@@ -3289,7 +3417,7 @@
         <v>1.0204081632653061</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>31</v>
       </c>
@@ -3309,11 +3437,11 @@
         <v>154.16</v>
       </c>
       <c r="H62" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>155.27166666666665</v>
       </c>
       <c r="I62" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.1370231565194842</v>
       </c>
       <c r="J62" s="24">
@@ -3329,7 +3457,7 @@
         <v>1.1459854014598541</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>41</v>
       </c>
@@ -3349,11 +3477,11 @@
         <v>202.70099999999999</v>
       </c>
       <c r="H63" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199.72400000000002</v>
       </c>
       <c r="I63" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2959712632552538</v>
       </c>
       <c r="J63" s="24">
@@ -3369,7 +3497,7 @@
         <v>1.4137931034482758</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>46</v>
       </c>
@@ -3389,11 +3517,11 @@
         <v>293.42099999999999</v>
       </c>
       <c r="H64" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>291.69366666666673</v>
       </c>
       <c r="I64" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.3334466966774796</v>
       </c>
       <c r="J64" s="24">
@@ -3429,11 +3557,11 @@
         <v>302.31299999999999</v>
       </c>
       <c r="H65" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>301.4976666666667</v>
       </c>
       <c r="I65" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4401111310474857</v>
       </c>
       <c r="J65" s="24">
@@ -3469,11 +3597,11 @@
         <v>262.49799999999999</v>
       </c>
       <c r="H66" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>260.30966666666671</v>
       </c>
       <c r="I66" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.2343541587071787</v>
       </c>
       <c r="J66" s="24">
@@ -3602,9 +3730,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="M1:O1"/>
-  </mergeCells>
+  <sortState ref="L68:M84">
+    <sortCondition ref="L68"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added an atomix tab to help with improving performance.
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozidar\Documents\Code\SDR\Ziria\compiler\code\WiFi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimitris\work\ZIRIA\Ziria\code\WiFi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28890" windowHeight="22185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Latest" sheetId="2" r:id="rId1"/>
-    <sheet name="TX Optim" sheetId="3" r:id="rId2"/>
-    <sheet name="Old" sheetId="1" r:id="rId3"/>
+    <sheet name="Atomix" sheetId="4" r:id="rId2"/>
+    <sheet name="TX Optim" sheetId="3" r:id="rId3"/>
+    <sheet name="Old" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="138">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -434,12 +435,18 @@
   </si>
   <si>
     <t>new-c-lib, 21/8/2015</t>
+  </si>
+  <si>
+    <t>BASELINE</t>
+  </si>
+  <si>
+    <t>SC-SC-OPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -865,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="N53" sqref="N53"/>
@@ -2272,7 +2279,7 @@
         <v>144.15299999999999</v>
       </c>
       <c r="N33">
-        <f>$M33/$G33</f>
+        <f t="shared" ref="N33:N49" si="4">$M33/$G33</f>
         <v>1.1155108105180072</v>
       </c>
     </row>
@@ -2303,7 +2310,7 @@
         <v>122.28800000000001</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" ref="I34:I66" si="4">$H34/$D34</f>
+        <f t="shared" ref="I34:I66" si="5">$H34/$D34</f>
         <v>1.1471992645196396</v>
       </c>
       <c r="J34" s="24">
@@ -2314,7 +2321,7 @@
         <v>128.56</v>
       </c>
       <c r="N34">
-        <f>$M34/$G34</f>
+        <f t="shared" si="4"/>
         <v>1.0199127330424436</v>
       </c>
     </row>
@@ -2345,18 +2352,18 @@
         <v>99.559833333333316</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1684713296058611</v>
       </c>
       <c r="J35" s="24">
-        <f t="shared" ref="J35:J42" si="5">$H35/$C35</f>
+        <f t="shared" ref="J35:J42" si="6">$H35/$C35</f>
         <v>0.8969354354354353</v>
       </c>
       <c r="M35">
         <v>103.568</v>
       </c>
       <c r="N35">
-        <f>$M35/$G35</f>
+        <f t="shared" si="4"/>
         <v>1.0324690213436212</v>
       </c>
     </row>
@@ -2387,18 +2394,18 @@
         <v>89.668099999999995</v>
       </c>
       <c r="I36" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2779058830236003</v>
       </c>
       <c r="J36" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.90573838383838379</v>
       </c>
       <c r="M36">
         <v>86.337100000000007</v>
       </c>
       <c r="N36">
-        <f>$M36/$G36</f>
+        <f t="shared" si="4"/>
         <v>0.94882607128413432</v>
       </c>
     </row>
@@ -2429,18 +2436,18 @@
         <v>66.846133333333327</v>
       </c>
       <c r="I37" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2077970807623624</v>
       </c>
       <c r="J37" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.96878454106280187</v>
       </c>
       <c r="M37">
         <v>68.238</v>
       </c>
       <c r="N37">
-        <f>$M37/$G37</f>
+        <f t="shared" si="4"/>
         <v>0.99806056989407732</v>
       </c>
     </row>
@@ -2471,18 +2478,18 @@
         <v>58.86343333333334</v>
       </c>
       <c r="I38" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3473716416862755</v>
       </c>
       <c r="J38" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98105722222222236</v>
       </c>
       <c r="M38">
         <v>57.339500000000001</v>
       </c>
       <c r="N38">
-        <f>$M38/$G38</f>
+        <f t="shared" si="4"/>
         <v>0.96892288766547363</v>
       </c>
     </row>
@@ -2513,18 +2520,18 @@
         <v>52.712699999999991</v>
       </c>
       <c r="I39" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5903185904784889</v>
       </c>
       <c r="J39" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1459282608695651</v>
       </c>
       <c r="M39">
         <v>53.083500000000001</v>
       </c>
       <c r="N39">
-        <f>$M39/$G39</f>
+        <f t="shared" si="4"/>
         <v>1.008193405391238</v>
       </c>
     </row>
@@ -2555,18 +2562,18 @@
         <v>55.797166666666669</v>
       </c>
       <c r="I40" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7710518826052504</v>
       </c>
       <c r="J40" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2399370370370371</v>
       </c>
       <c r="M40">
         <v>55.146500000000003</v>
       </c>
       <c r="N40">
-        <f>$M40/$G40</f>
+        <f t="shared" si="4"/>
         <v>0.9850421281832813</v>
       </c>
     </row>
@@ -2597,18 +2604,18 @@
         <v>259.80500000000001</v>
       </c>
       <c r="I41" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0520976755487164</v>
       </c>
       <c r="J41" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.89897923875432528</v>
       </c>
       <c r="M41">
         <v>245.54300000000001</v>
       </c>
       <c r="N41">
-        <f>$M41/$G41</f>
+        <f t="shared" si="4"/>
         <v>0.94485040885040883</v>
       </c>
     </row>
@@ -2639,18 +2646,18 @@
         <v>56.271433333333334</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5623359015293492</v>
       </c>
       <c r="J42" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0420635802469136</v>
       </c>
       <c r="M42">
         <v>65.837800000000001</v>
       </c>
       <c r="N42">
-        <f>$M42/$G42</f>
+        <f t="shared" si="4"/>
         <v>1.1695993490955021</v>
       </c>
     </row>
@@ -2681,18 +2688,18 @@
         <v>78.3018</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6966693607625518</v>
       </c>
       <c r="J43" s="24">
-        <f t="shared" ref="J43:J66" si="6">$H43/$C43</f>
+        <f t="shared" ref="J43:J66" si="7">$H43/$C43</f>
         <v>1.0169064935064935</v>
       </c>
       <c r="M43">
         <v>90.422499999999999</v>
       </c>
       <c r="N43">
-        <f>$M43/$G43</f>
+        <f t="shared" si="4"/>
         <v>1.1487137987938965</v>
       </c>
     </row>
@@ -2723,18 +2730,18 @@
         <v>102.73433333333332</v>
       </c>
       <c r="I44" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3009066917509338</v>
       </c>
       <c r="J44" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0483095238095237</v>
       </c>
       <c r="M44">
         <v>123.629</v>
       </c>
       <c r="N44">
-        <f>$M44/$G44</f>
+        <f t="shared" si="4"/>
         <v>1.2030731503196739</v>
       </c>
     </row>
@@ -2765,18 +2772,18 @@
         <v>134.68733333333333</v>
       </c>
       <c r="I45" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4323779287145708</v>
       </c>
       <c r="J45" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.98311922141119212</v>
       </c>
       <c r="M45">
         <v>157.97</v>
       </c>
       <c r="N45">
-        <f>$M45/$G45</f>
+        <f t="shared" si="4"/>
         <v>1.1706337443680341</v>
       </c>
     </row>
@@ -2807,18 +2814,18 @@
         <v>184.19333333333336</v>
       </c>
       <c r="I46" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3968780294689531</v>
       </c>
       <c r="J46" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2702988505747128</v>
       </c>
       <c r="M46">
         <v>208.244</v>
       </c>
       <c r="N46">
-        <f>$M46/$G46</f>
+        <f t="shared" si="4"/>
         <v>1.1323578190676606</v>
       </c>
     </row>
@@ -2849,18 +2856,18 @@
         <v>215.55499999999998</v>
       </c>
       <c r="I47" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3467427655828366</v>
       </c>
       <c r="J47" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0777749999999999</v>
       </c>
       <c r="M47">
         <v>240.614</v>
       </c>
       <c r="N47">
-        <f>$M47/$G47</f>
+        <f t="shared" si="4"/>
         <v>1.1081053698074976</v>
       </c>
     </row>
@@ -2891,11 +2898,11 @@
         <v>231.59933333333333</v>
       </c>
       <c r="I48" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1643097013471717</v>
       </c>
       <c r="J48" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0025945165945167</v>
       </c>
       <c r="K48" s="18"/>
@@ -2903,7 +2910,7 @@
         <v>233.05799999999999</v>
       </c>
       <c r="N48">
-        <f>$M48/$G48</f>
+        <f t="shared" si="4"/>
         <v>1.0065647971391305</v>
       </c>
     </row>
@@ -2934,18 +2941,18 @@
         <v>202.96966666666665</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4492312276283354</v>
       </c>
       <c r="J49" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.79285026041666662</v>
       </c>
       <c r="M49">
         <v>226.64099999999999</v>
       </c>
       <c r="N49">
-        <f>$M49/$G49</f>
+        <f t="shared" si="4"/>
         <v>1.1133867164472391</v>
       </c>
     </row>
@@ -2973,11 +2980,11 @@
         <v>195.28633333333332</v>
       </c>
       <c r="I50" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1916277158768707</v>
       </c>
       <c r="J50" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0278228070175437</v>
       </c>
       <c r="K50" s="27">
@@ -3013,19 +3020,19 @@
         <v>199.39166666666665</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2163220073608654</v>
       </c>
       <c r="J51" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0494298245614033</v>
       </c>
       <c r="K51" s="27">
-        <f t="shared" ref="K51:K66" si="7">$H51/$H34</f>
+        <f t="shared" ref="K51:K66" si="8">$H51/$H34</f>
         <v>1.6305088534170697</v>
       </c>
       <c r="L51" s="27">
-        <f t="shared" ref="L51:L66" si="8">$C51/$C34</f>
+        <f t="shared" ref="L51:L66" si="9">$C51/$C34</f>
         <v>1.3475177304964538</v>
       </c>
     </row>
@@ -3053,11 +3060,11 @@
         <v>180.9193333333333</v>
       </c>
       <c r="I52" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3943471648478118</v>
       </c>
       <c r="J52" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0338247619047618</v>
       </c>
       <c r="K52" s="15">
@@ -3065,7 +3072,7 @@
         <v>1.8171920068166714</v>
       </c>
       <c r="L52" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5765765765765767</v>
       </c>
     </row>
@@ -3093,19 +3100,19 @@
         <v>135.66499999999999</v>
       </c>
       <c r="I53" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2714024647392344</v>
       </c>
       <c r="J53" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.77522857142857138</v>
       </c>
       <c r="K53" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5129683800593523</v>
       </c>
       <c r="L53" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.7676767676767677</v>
       </c>
     </row>
@@ -3133,19 +3140,19 @@
         <v>108.074</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4347198105342529</v>
       </c>
       <c r="J54" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1620860215053763</v>
       </c>
       <c r="K54" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6167576883030883</v>
       </c>
       <c r="L54" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3478260869565217</v>
       </c>
     </row>
@@ -3173,19 +3180,19 @@
         <v>86.069833333333335</v>
       </c>
       <c r="I55" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4413653280101908</v>
       </c>
       <c r="J55" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1790388127853881</v>
       </c>
       <c r="K55" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4621952621406724</v>
       </c>
       <c r="L55" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2166666666666666</v>
       </c>
     </row>
@@ -3213,19 +3220,19 @@
         <v>80.540199999999999</v>
       </c>
       <c r="I56" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8800057889282078</v>
       </c>
       <c r="J56" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5792196078431373</v>
       </c>
       <c r="K56" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5279088341139804</v>
       </c>
       <c r="L56" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1086956521739131</v>
       </c>
     </row>
@@ -3253,19 +3260,19 @@
         <v>86.34996666666666</v>
       </c>
       <c r="I57" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.163487203642644</v>
       </c>
       <c r="J57" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6931366013071893</v>
       </c>
       <c r="K57" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5475690223219218</v>
       </c>
       <c r="L57" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1333333333333333</v>
       </c>
     </row>
@@ -3290,7 +3297,7 @@
         <v>34.685566666666666</v>
       </c>
       <c r="I58" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.15912927254848885</v>
       </c>
       <c r="J58" s="24"/>
@@ -3321,19 +3328,19 @@
         <v>51.380766666666666</v>
       </c>
       <c r="I59" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1101745758402708</v>
       </c>
       <c r="J59" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0276153333333333</v>
       </c>
       <c r="K59" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.91308793153186663</v>
       </c>
       <c r="L59" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.92592592592592593</v>
       </c>
     </row>
@@ -3361,19 +3368,19 @@
         <v>76.121200000000002</v>
       </c>
       <c r="I60" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2882683455185486</v>
       </c>
       <c r="J60" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0286648648648649</v>
       </c>
       <c r="K60" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.97215134262558467</v>
       </c>
       <c r="L60" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.96103896103896103</v>
       </c>
     </row>
@@ -3401,19 +3408,19 @@
         <v>104.13466666666666</v>
       </c>
       <c r="I61" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3835988524690226</v>
       </c>
       <c r="J61" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0413466666666666</v>
       </c>
       <c r="K61" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0136306265675545</v>
       </c>
       <c r="L61" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0204081632653061</v>
       </c>
     </row>
@@ -3441,19 +3448,19 @@
         <v>155.27166666666665</v>
       </c>
       <c r="I62" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1370231565194842</v>
       </c>
       <c r="J62" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.98899150743099773</v>
       </c>
       <c r="K62" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1528305062094431</v>
       </c>
       <c r="L62" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1459854014598541</v>
       </c>
     </row>
@@ -3481,19 +3488,19 @@
         <v>199.72400000000002</v>
       </c>
       <c r="I63" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.2959712632552538</v>
       </c>
       <c r="J63" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.97426341463414645</v>
       </c>
       <c r="K63" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.084317202938941</v>
       </c>
       <c r="L63" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.4137931034482758</v>
       </c>
     </row>
@@ -3521,19 +3528,19 @@
         <v>291.69366666666673</v>
       </c>
       <c r="I64" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3334466966774796</v>
       </c>
       <c r="J64" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.99895091324200935</v>
       </c>
       <c r="K64" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.3532215289214666</v>
       </c>
       <c r="L64" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.46</v>
       </c>
     </row>
@@ -3561,19 +3568,19 @@
         <v>301.4976666666667</v>
       </c>
       <c r="I65" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.4401111310474857</v>
       </c>
       <c r="J65" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.75374416666666677</v>
       </c>
       <c r="K65" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.3018071439468739</v>
       </c>
       <c r="L65" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.7316017316017316</v>
       </c>
     </row>
@@ -3601,19 +3608,19 @@
         <v>260.30966666666671</v>
       </c>
       <c r="I66" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.2343541587071787</v>
       </c>
       <c r="J66" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.57846592592592605</v>
       </c>
       <c r="K66" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.282505267617986</v>
       </c>
       <c r="L66" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.7578125</v>
       </c>
     </row>
@@ -3739,6 +3746,222 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>63.415999999999997</v>
+      </c>
+      <c r="C2">
+        <v>79.016199999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>31.994</v>
+      </c>
+      <c r="C3">
+        <v>38.157499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>40.762700000000002</v>
+      </c>
+      <c r="C4">
+        <v>126.254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>140.99799999999999</v>
+      </c>
+      <c r="C5">
+        <v>202.429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>40.002400000000002</v>
+      </c>
+      <c r="C6">
+        <v>39.424100000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>92.693399999999997</v>
+      </c>
+      <c r="C7">
+        <v>28.790400000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>25.4939</v>
+      </c>
+      <c r="C8">
+        <v>79.364999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <v>70.402500000000003</v>
+      </c>
+      <c r="C9">
+        <v>97.892099999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>79.056799999999996</v>
+      </c>
+      <c r="C10">
+        <v>48.375900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>38.575299999999999</v>
+      </c>
+      <c r="C11">
+        <v>114.246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>82.602599999999995</v>
+      </c>
+      <c r="C12">
+        <v>48.1678</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>92.458799999999997</v>
+      </c>
+      <c r="C13">
+        <v>148.13300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>68.573800000000006</v>
+      </c>
+      <c r="C14">
+        <v>96.390699999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>111.008</v>
+      </c>
+      <c r="C15">
+        <v>165.69800000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>48.226300000000002</v>
+      </c>
+      <c r="C16">
+        <v>61.790999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <v>63.304099999999998</v>
+      </c>
+      <c r="C17">
+        <v>82.345399999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>72.156400000000005</v>
+      </c>
+      <c r="C18">
+        <v>88.995800000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T66"/>
   <sheetViews>
@@ -7523,7 +7746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R66"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding non-atomix baseline in perf results.
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="139">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>SC-SC-OPT</t>
+  </si>
+  <si>
+    <t>Non-Atomix</t>
   </si>
 </sst>
 </file>
@@ -3747,211 +3750,266 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B2">
+        <v>141.738</v>
+      </c>
+      <c r="C2">
         <v>63.415999999999997</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>79.016199999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B3">
+        <v>83.485799999999998</v>
+      </c>
+      <c r="C3">
         <v>31.994</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>38.157499999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B4">
+        <v>130.785</v>
+      </c>
+      <c r="C4">
         <v>40.762700000000002</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>126.254</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B5">
+        <v>234.142</v>
+      </c>
+      <c r="C5">
         <v>140.99799999999999</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>202.429</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B6">
+        <v>50.476500000000001</v>
+      </c>
+      <c r="C6">
         <v>40.002400000000002</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>39.424100000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B7">
+        <v>60.640500000000003</v>
+      </c>
+      <c r="C7">
         <v>92.693399999999997</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>28.790400000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B8">
+        <v>99.204300000000003</v>
+      </c>
+      <c r="C8">
         <v>25.4939</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>79.364999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B9">
+        <v>221.26400000000001</v>
+      </c>
+      <c r="C9">
         <v>70.402500000000003</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>97.892099999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B10">
+        <v>53.211399999999998</v>
+      </c>
+      <c r="C10">
         <v>79.056799999999996</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>48.375900000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B11">
+        <v>119.5</v>
+      </c>
+      <c r="C11">
         <v>38.575299999999999</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>114.246</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B12">
+        <v>50.630499999999998</v>
+      </c>
+      <c r="C12">
         <v>82.602599999999995</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>48.1678</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
         <v>41</v>
       </c>
       <c r="B13">
+        <v>197.06899999999999</v>
+      </c>
+      <c r="C13">
         <v>92.458799999999997</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>148.13300000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B14">
+        <v>112.996</v>
+      </c>
+      <c r="C14">
         <v>68.573800000000006</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>96.390699999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
       <c r="B15">
+        <v>230.12200000000001</v>
+      </c>
+      <c r="C15">
         <v>111.008</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>165.69800000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B16">
+        <v>67.674700000000001</v>
+      </c>
+      <c r="C16">
         <v>48.226300000000002</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>61.790999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B17">
+        <v>84.192999999999998</v>
+      </c>
+      <c r="C17">
         <v>63.304099999999998</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>82.345399999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B18">
+        <v>234.87899999999999</v>
+      </c>
+      <c r="C18">
         <v>72.156400000000005</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>88.995800000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrections to perf numbers.
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -3753,7 +3753,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,139 +3777,139 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B2">
-        <v>141.738</v>
+        <v>83.485799999999998</v>
       </c>
       <c r="C2">
-        <v>63.415999999999997</v>
+        <v>31.994</v>
       </c>
       <c r="D2">
-        <v>79.016199999999998</v>
+        <v>38.157499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B3">
-        <v>83.485799999999998</v>
+        <v>60.640500000000003</v>
       </c>
       <c r="C3">
-        <v>31.994</v>
+        <v>25.4939</v>
       </c>
       <c r="D3">
-        <v>38.157499999999999</v>
+        <v>28.790400000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4">
-        <v>130.785</v>
+        <v>221.26400000000001</v>
       </c>
       <c r="C4">
-        <v>40.762700000000002</v>
+        <v>79.056799999999996</v>
       </c>
       <c r="D4">
-        <v>126.254</v>
+        <v>97.892099999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>234.142</v>
+        <v>230.12200000000001</v>
       </c>
       <c r="C5">
-        <v>140.99799999999999</v>
+        <v>111.008</v>
       </c>
       <c r="D5">
-        <v>202.429</v>
+        <v>165.69800000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>50.476500000000001</v>
+        <v>234.87899999999999</v>
       </c>
       <c r="C6">
-        <v>40.002400000000002</v>
+        <v>72.156400000000005</v>
       </c>
       <c r="D6">
-        <v>39.424100000000003</v>
+        <v>88.995800000000003</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7">
-        <v>60.640500000000003</v>
+        <v>197.06899999999999</v>
       </c>
       <c r="C7">
-        <v>92.693399999999997</v>
+        <v>92.458799999999997</v>
       </c>
       <c r="D7">
-        <v>28.790400000000002</v>
+        <v>148.13300000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>99.204300000000003</v>
+        <v>141.738</v>
       </c>
       <c r="C8">
-        <v>25.4939</v>
+        <v>63.415999999999997</v>
       </c>
       <c r="D8">
-        <v>79.364999999999995</v>
+        <v>79.016199999999998</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>221.26400000000001</v>
+        <v>112.996</v>
       </c>
       <c r="C9">
-        <v>70.402500000000003</v>
+        <v>68.573800000000006</v>
       </c>
       <c r="D9">
-        <v>97.892099999999999</v>
+        <v>96.390699999999995</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>53.211399999999998</v>
+        <v>234.142</v>
       </c>
       <c r="C10">
-        <v>79.056799999999996</v>
+        <v>140.99799999999999</v>
       </c>
       <c r="D10">
-        <v>48.375900000000001</v>
+        <v>202.429</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>119.5</v>
       </c>
       <c r="C11">
-        <v>38.575299999999999</v>
+        <v>82.602599999999995</v>
       </c>
       <c r="D11">
         <v>114.246</v>
@@ -3917,58 +3917,58 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B12">
-        <v>50.630499999999998</v>
+        <v>130.785</v>
       </c>
       <c r="C12">
-        <v>82.602599999999995</v>
+        <v>92.693399999999997</v>
       </c>
       <c r="D12">
-        <v>48.1678</v>
+        <v>126.254</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13">
-        <v>197.06899999999999</v>
+        <v>50.476500000000001</v>
       </c>
       <c r="C13">
-        <v>92.458799999999997</v>
+        <v>40.002400000000002</v>
       </c>
       <c r="D13">
-        <v>148.13300000000001</v>
+        <v>39.424100000000003</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B14">
-        <v>112.996</v>
+        <v>50.630499999999998</v>
       </c>
       <c r="C14">
-        <v>68.573800000000006</v>
+        <v>38.575299999999999</v>
       </c>
       <c r="D14">
-        <v>96.390699999999995</v>
+        <v>48.1678</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B15">
-        <v>230.12200000000001</v>
+        <v>53.211399999999998</v>
       </c>
       <c r="C15">
-        <v>111.008</v>
+        <v>40.762700000000002</v>
       </c>
       <c r="D15">
-        <v>165.69800000000001</v>
+        <v>48.375900000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4001,16 +4001,16 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B18">
-        <v>234.87899999999999</v>
+        <v>99.204300000000003</v>
       </c>
       <c r="C18">
-        <v>72.156400000000005</v>
+        <v>70.402500000000003</v>
       </c>
       <c r="D18">
-        <v>88.995800000000003</v>
+        <v>79.364999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atomix perf updates.Nothing finalized yet.
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="142">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>unsound ts_get() without memcopy()</t>
+  </si>
+  <si>
+    <t>new API</t>
+  </si>
+  <si>
+    <t>new API (no mitig copy)</t>
   </si>
 </sst>
 </file>
@@ -3841,22 +3847,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="53.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>138</v>
       </c>
@@ -3864,13 +3871,19 @@
         <v>136</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>45</v>
       </c>
@@ -3881,13 +3894,19 @@
         <v>31.994</v>
       </c>
       <c r="D2">
+        <v>73</v>
+      </c>
+      <c r="E2">
+        <v>73</v>
+      </c>
+      <c r="F2">
         <v>38.157499999999999</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>48.465800000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>38</v>
       </c>
@@ -3898,13 +3917,19 @@
         <v>25.4939</v>
       </c>
       <c r="D3">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
         <v>28.790400000000002</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>41.415300000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>34</v>
       </c>
@@ -3915,13 +3940,19 @@
         <v>79.056799999999996</v>
       </c>
       <c r="D4">
+        <v>191</v>
+      </c>
+      <c r="E4">
+        <v>185</v>
+      </c>
+      <c r="F4">
         <v>97.892099999999999</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>117.271</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>32</v>
       </c>
@@ -3932,13 +3963,19 @@
         <v>111.008</v>
       </c>
       <c r="D5">
+        <v>206</v>
+      </c>
+      <c r="E5">
+        <v>204</v>
+      </c>
+      <c r="F5">
         <v>165.69800000000001</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>183.40199999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>46</v>
       </c>
@@ -3949,13 +3986,19 @@
         <v>72.156400000000005</v>
       </c>
       <c r="D6">
+        <v>185</v>
+      </c>
+      <c r="E6">
+        <v>176</v>
+      </c>
+      <c r="F6">
         <v>88.995800000000003</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>117.873</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>41</v>
       </c>
@@ -3966,13 +4009,19 @@
         <v>92.458799999999997</v>
       </c>
       <c r="D7">
+        <v>163</v>
+      </c>
+      <c r="E7">
+        <v>166</v>
+      </c>
+      <c r="F7">
         <v>148.13300000000001</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>154.893</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
@@ -3983,13 +4032,19 @@
         <v>63.415999999999997</v>
       </c>
       <c r="D8">
+        <v>126</v>
+      </c>
+      <c r="E8">
+        <v>127</v>
+      </c>
+      <c r="F8">
         <v>79.016199999999998</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>91.993099999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>39</v>
       </c>
@@ -4000,13 +4055,19 @@
         <v>68.573800000000006</v>
       </c>
       <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>101</v>
+      </c>
+      <c r="F9">
         <v>96.390699999999995</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>100.99299999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>35</v>
       </c>
@@ -4017,13 +4078,19 @@
         <v>140.99799999999999</v>
       </c>
       <c r="D10">
+        <v>196</v>
+      </c>
+      <c r="E10">
+        <v>172</v>
+      </c>
+      <c r="F10">
         <v>202.429</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>230.75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>36</v>
       </c>
@@ -4034,13 +4101,19 @@
         <v>82.602599999999995</v>
       </c>
       <c r="D11">
+        <v>111</v>
+      </c>
+      <c r="E11">
+        <v>105</v>
+      </c>
+      <c r="F11">
         <v>114.246</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>118.363</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>47</v>
       </c>
@@ -4051,13 +4124,19 @@
         <v>92.693399999999997</v>
       </c>
       <c r="D12">
+        <v>127</v>
+      </c>
+      <c r="E12">
+        <v>123</v>
+      </c>
+      <c r="F12">
         <v>126.254</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>136.48500000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>37</v>
       </c>
@@ -4068,13 +4147,19 @@
         <v>40.002400000000002</v>
       </c>
       <c r="D13">
+        <v>47</v>
+      </c>
+      <c r="E13">
+        <v>48</v>
+      </c>
+      <c r="F13">
         <v>39.424100000000003</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>51.6723</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>33</v>
       </c>
@@ -4085,13 +4170,19 @@
         <v>38.575299999999999</v>
       </c>
       <c r="D14">
+        <v>47</v>
+      </c>
+      <c r="E14">
+        <v>47</v>
+      </c>
+      <c r="F14">
         <v>48.1678</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>50.582299999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>40</v>
       </c>
@@ -4102,13 +4193,19 @@
         <v>40.762700000000002</v>
       </c>
       <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>47</v>
+      </c>
+      <c r="F15">
         <v>48.375900000000001</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>53.897199999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>43</v>
       </c>
@@ -4119,13 +4216,19 @@
         <v>48.226300000000002</v>
       </c>
       <c r="D16">
+        <v>62</v>
+      </c>
+      <c r="E16">
+        <v>58</v>
+      </c>
+      <c r="F16">
         <v>61.790999999999997</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>64.622500000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>44</v>
       </c>
@@ -4136,13 +4239,19 @@
         <v>63.304099999999998</v>
       </c>
       <c r="D17">
+        <v>80</v>
+      </c>
+      <c r="E17">
+        <v>78</v>
+      </c>
+      <c r="F17">
         <v>82.345399999999998</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>84.139700000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>42</v>
       </c>
@@ -4153,9 +4262,15 @@
         <v>70.402500000000003</v>
       </c>
       <c r="D18">
+        <v>92</v>
+      </c>
+      <c r="E18">
+        <v>89</v>
+      </c>
+      <c r="F18">
         <v>79.364999999999995</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>95.824799999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new perf results
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimitris\work\ZIRIA\Ziria\code\WiFi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozidar\Documents\Code\SDR\Ziria\compiler\code\WiFi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="TX Optim" sheetId="3" r:id="rId3"/>
     <sheet name="Old" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="145">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -453,12 +453,21 @@
   </si>
   <si>
     <t>new API (no mitig copy)</t>
+  </si>
+  <si>
+    <t>2 threads, multiple runs</t>
+  </si>
+  <si>
+    <t>2 threads, avg</t>
+  </si>
+  <si>
+    <t>2Th/1Th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -556,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -602,6 +611,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3847,10 +3859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3858,9 +3870,10 @@
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3885,186 +3898,186 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2">
-        <v>83.485799999999998</v>
+        <v>130.785</v>
       </c>
       <c r="C2">
-        <v>31.994</v>
+        <v>92.693399999999997</v>
       </c>
       <c r="D2">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="E2">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="F2">
-        <v>38.157499999999999</v>
+        <v>126.254</v>
       </c>
       <c r="G2">
-        <v>48.465800000000002</v>
+        <v>136.48500000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3">
-        <v>60.640500000000003</v>
+        <v>119.5</v>
       </c>
       <c r="C3">
-        <v>25.4939</v>
+        <v>82.602599999999995</v>
       </c>
       <c r="D3">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="E3">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="F3">
-        <v>28.790400000000002</v>
+        <v>114.246</v>
       </c>
       <c r="G3">
-        <v>41.415300000000002</v>
+        <v>118.363</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B4">
-        <v>221.26400000000001</v>
+        <v>99.204300000000003</v>
       </c>
       <c r="C4">
-        <v>79.056799999999996</v>
+        <v>70.402500000000003</v>
       </c>
       <c r="D4">
-        <v>191</v>
+        <v>92</v>
       </c>
       <c r="E4">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="F4">
-        <v>97.892099999999999</v>
+        <v>79.364999999999995</v>
       </c>
       <c r="G4">
-        <v>117.271</v>
+        <v>95.824799999999996</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B5">
-        <v>230.12200000000001</v>
+        <v>84.192999999999998</v>
       </c>
       <c r="C5">
-        <v>111.008</v>
+        <v>63.304099999999998</v>
       </c>
       <c r="D5">
-        <v>206</v>
+        <v>80</v>
       </c>
       <c r="E5">
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="F5">
-        <v>165.69800000000001</v>
+        <v>82.345399999999998</v>
       </c>
       <c r="G5">
-        <v>183.40199999999999</v>
+        <v>84.139700000000005</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6">
-        <v>234.87899999999999</v>
+        <v>67.674700000000001</v>
       </c>
       <c r="C6">
-        <v>72.156400000000005</v>
+        <v>48.226300000000002</v>
       </c>
       <c r="D6">
-        <v>185</v>
+        <v>62</v>
       </c>
       <c r="E6">
-        <v>176</v>
+        <v>58</v>
       </c>
       <c r="F6">
-        <v>88.995800000000003</v>
+        <v>61.790999999999997</v>
       </c>
       <c r="G6">
-        <v>117.873</v>
+        <v>64.622500000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>197.06899999999999</v>
+        <v>53.211399999999998</v>
       </c>
       <c r="C7">
-        <v>92.458799999999997</v>
+        <v>40.762700000000002</v>
       </c>
       <c r="D7">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="E7">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="F7">
-        <v>148.13300000000001</v>
+        <v>48.375900000000001</v>
       </c>
       <c r="G7">
-        <v>154.893</v>
+        <v>53.897199999999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>141.738</v>
+        <v>50.630499999999998</v>
       </c>
       <c r="C8">
-        <v>63.415999999999997</v>
+        <v>38.575299999999999</v>
       </c>
       <c r="D8">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="E8">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="F8">
-        <v>79.016199999999998</v>
+        <v>48.1678</v>
       </c>
       <c r="G8">
-        <v>91.993099999999998</v>
+        <v>50.582299999999996</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9">
-        <v>112.996</v>
+        <v>50.476500000000001</v>
       </c>
       <c r="C9">
-        <v>68.573800000000006</v>
+        <v>40.002400000000002</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="E9">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="F9">
-        <v>96.390699999999995</v>
+        <v>39.424100000000003</v>
       </c>
       <c r="G9">
-        <v>100.99299999999999</v>
+        <v>51.6723</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,189 +4105,1042 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>119.5</v>
+        <v>60.640500000000003</v>
       </c>
       <c r="C11">
-        <v>82.602599999999995</v>
+        <v>25.4939</v>
       </c>
       <c r="D11">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="E11">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="F11">
-        <v>114.246</v>
+        <v>28.790400000000002</v>
       </c>
       <c r="G11">
-        <v>118.363</v>
+        <v>41.415300000000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12">
-        <v>130.785</v>
+        <v>83.485799999999998</v>
       </c>
       <c r="C12">
-        <v>92.693399999999997</v>
+        <v>31.994</v>
       </c>
       <c r="D12">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="E12">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="F12">
-        <v>126.254</v>
+        <v>38.157499999999999</v>
       </c>
       <c r="G12">
-        <v>136.48500000000001</v>
+        <v>48.465800000000002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13">
-        <v>50.476500000000001</v>
+        <v>112.996</v>
       </c>
       <c r="C13">
-        <v>40.002400000000002</v>
+        <v>68.573800000000006</v>
       </c>
       <c r="D13">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E13">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="F13">
-        <v>39.424100000000003</v>
+        <v>96.390699999999995</v>
       </c>
       <c r="G13">
-        <v>51.6723</v>
+        <v>100.99299999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14">
-        <v>50.630499999999998</v>
+        <v>141.738</v>
       </c>
       <c r="C14">
-        <v>38.575299999999999</v>
+        <v>63.415999999999997</v>
       </c>
       <c r="D14">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="E14">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="F14">
-        <v>48.1678</v>
+        <v>79.016199999999998</v>
       </c>
       <c r="G14">
-        <v>50.582299999999996</v>
+        <v>91.993099999999998</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15">
-        <v>53.211399999999998</v>
+        <v>197.06899999999999</v>
       </c>
       <c r="C15">
-        <v>40.762700000000002</v>
+        <v>92.458799999999997</v>
       </c>
       <c r="D15">
-        <v>50</v>
+        <v>163</v>
       </c>
       <c r="E15">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="F15">
-        <v>48.375900000000001</v>
+        <v>148.13300000000001</v>
       </c>
       <c r="G15">
-        <v>53.897199999999998</v>
+        <v>154.893</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>234.87899999999999</v>
+      </c>
+      <c r="C16">
+        <v>72.156400000000005</v>
+      </c>
+      <c r="D16">
+        <v>185</v>
+      </c>
+      <c r="E16">
+        <v>176</v>
+      </c>
+      <c r="F16">
+        <v>88.995800000000003</v>
+      </c>
+      <c r="G16">
+        <v>117.873</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>230.12200000000001</v>
+      </c>
+      <c r="C17">
+        <v>111.008</v>
+      </c>
+      <c r="D17">
+        <v>206</v>
+      </c>
+      <c r="E17">
+        <v>204</v>
+      </c>
+      <c r="F17">
+        <v>165.69800000000001</v>
+      </c>
+      <c r="G17">
+        <v>183.40199999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>221.26400000000001</v>
+      </c>
+      <c r="C18">
+        <v>79.056799999999996</v>
+      </c>
+      <c r="D18">
+        <v>191</v>
+      </c>
+      <c r="E18">
+        <v>185</v>
+      </c>
+      <c r="F18">
+        <v>97.892099999999999</v>
+      </c>
+      <c r="G18">
+        <v>117.271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28">
+        <v>213.352</v>
+      </c>
+      <c r="C28">
+        <v>220.76300000000001</v>
+      </c>
+      <c r="D28">
+        <v>206.48699999999999</v>
+      </c>
+      <c r="E28">
+        <v>213.36500000000001</v>
+      </c>
+      <c r="F28">
+        <v>220.71799999999999</v>
+      </c>
+      <c r="G28">
+        <f>AVERAGE(B28:F28)</f>
+        <v>214.93699999999998</v>
+      </c>
+      <c r="H28">
+        <f>$G28/$G46</f>
+        <v>1.3567148031303218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>188.26</v>
+      </c>
+      <c r="C29">
+        <v>182.893</v>
+      </c>
+      <c r="D29">
+        <v>188.25700000000001</v>
+      </c>
+      <c r="E29">
+        <v>177.80799999999999</v>
+      </c>
+      <c r="F29">
+        <v>188.26900000000001</v>
+      </c>
+      <c r="G29">
+        <f>AVERAGE(B29:F29)</f>
+        <v>185.09740000000002</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:H43" si="0">$G29/$G47</f>
+        <v>1.3440690938189381</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>139.143</v>
+      </c>
+      <c r="C30">
+        <v>145.465</v>
+      </c>
+      <c r="D30">
+        <v>136.184</v>
+      </c>
+      <c r="E30">
+        <v>142.24199999999999</v>
+      </c>
+      <c r="F30">
+        <v>136.191</v>
+      </c>
+      <c r="G30">
+        <f>AVERAGE(B30:F30)</f>
+        <v>139.845</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1.2584748736980595</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <v>120.76300000000001</v>
+      </c>
+      <c r="C31">
+        <v>125.505</v>
+      </c>
+      <c r="D31">
+        <v>123.09</v>
+      </c>
+      <c r="E31">
+        <v>116.37</v>
+      </c>
+      <c r="F31">
+        <v>120.762</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:G43" si="1">AVERAGE(B31:F31)</f>
+        <v>121.298</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>1.2282784537977418</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B16">
-        <v>67.674700000000001</v>
-      </c>
-      <c r="C16">
-        <v>48.226300000000002</v>
-      </c>
-      <c r="D16">
-        <v>62</v>
-      </c>
-      <c r="E16">
-        <v>58</v>
-      </c>
-      <c r="F16">
-        <v>61.790999999999997</v>
-      </c>
-      <c r="G16">
-        <v>64.622500000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="B32">
+        <v>98.470200000000006</v>
+      </c>
+      <c r="C32">
+        <v>98.468299999999999</v>
+      </c>
+      <c r="D32">
+        <v>99.999200000000002</v>
+      </c>
+      <c r="E32">
+        <v>100.005</v>
+      </c>
+      <c r="F32">
+        <v>98.466499999999996</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>99.08184</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>1.3931042899447803</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>79.811800000000005</v>
+      </c>
+      <c r="C33">
+        <v>82.0578</v>
+      </c>
+      <c r="D33">
+        <v>81.016199999999998</v>
+      </c>
+      <c r="E33">
+        <v>82.055899999999994</v>
+      </c>
+      <c r="F33">
+        <v>79.016900000000007</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>80.791719999999998</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>1.3531772776910553</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>75.296899999999994</v>
+      </c>
+      <c r="C34">
+        <v>76.194400000000002</v>
+      </c>
+      <c r="D34">
+        <v>77.090199999999996</v>
+      </c>
+      <c r="E34">
+        <v>76.197100000000006</v>
+      </c>
+      <c r="F34">
+        <v>78.053299999999993</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>76.566379999999995</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>1.3821724004471108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>77.111900000000006</v>
+      </c>
+      <c r="C35">
+        <v>80.683999999999997</v>
+      </c>
+      <c r="D35">
+        <v>80.017700000000005</v>
+      </c>
+      <c r="E35">
+        <v>82.054599999999994</v>
+      </c>
+      <c r="F35">
+        <v>82.0565</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>80.38494</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>1.4155692482165594</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>61.542700000000004</v>
+      </c>
+      <c r="C36">
+        <v>59.261200000000002</v>
+      </c>
+      <c r="D36">
+        <v>60.379899999999999</v>
+      </c>
+      <c r="E36">
+        <v>61.539499999999997</v>
+      </c>
+      <c r="F36">
+        <v>63.367400000000004</v>
+      </c>
+      <c r="G36">
+        <f>AVERAGE(B36:F36)</f>
+        <v>61.218139999999991</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>1.0406547654664831</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>92.754800000000003</v>
+      </c>
+      <c r="C37">
+        <v>98.465500000000006</v>
+      </c>
+      <c r="D37">
+        <v>96.975300000000004</v>
+      </c>
+      <c r="E37">
+        <v>98.466399999999993</v>
+      </c>
+      <c r="F37">
+        <v>94.122500000000002</v>
+      </c>
+      <c r="G37">
+        <f>AVERAGE(B37:F37)</f>
+        <v>96.156900000000007</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>1.1506384597987516</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>128.024</v>
+      </c>
+      <c r="C38">
+        <v>133.34200000000001</v>
+      </c>
+      <c r="D38">
+        <v>133.346</v>
+      </c>
+      <c r="E38">
+        <v>133.36500000000001</v>
+      </c>
+      <c r="F38">
+        <v>130.61000000000001</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>131.73740000000001</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>1.3115760469269548</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <v>193.94800000000001</v>
+      </c>
+      <c r="C39">
+        <v>200.01599999999999</v>
+      </c>
+      <c r="D39">
+        <v>193.935</v>
+      </c>
+      <c r="E39">
+        <v>206.47</v>
+      </c>
+      <c r="F39">
+        <v>193.958</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>197.66540000000001</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>1.4664040475978517</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>290.95600000000002</v>
+      </c>
+      <c r="C40">
+        <v>290.94</v>
+      </c>
+      <c r="D40">
+        <v>290.99299999999999</v>
+      </c>
+      <c r="E40">
+        <v>266.69099999999997</v>
+      </c>
+      <c r="F40">
+        <v>278.3</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>283.57599999999996</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>1.5977840983362706</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>336.91399999999999</v>
+      </c>
+      <c r="C41">
+        <v>304.83600000000001</v>
+      </c>
+      <c r="D41">
+        <v>336.90699999999998</v>
+      </c>
+      <c r="E41">
+        <v>320.04500000000002</v>
+      </c>
+      <c r="F41">
+        <v>355.62</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>330.86440000000005</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>1.4236923770690728</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>336.89699999999999</v>
+      </c>
+      <c r="C42">
+        <v>376.53199999999998</v>
+      </c>
+      <c r="D42">
+        <v>376.61799999999999</v>
+      </c>
+      <c r="E42">
+        <v>400.09800000000001</v>
+      </c>
+      <c r="F42">
+        <v>426.73899999999998</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>383.3768</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>1.8048446581556705</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43">
+        <v>355.74400000000003</v>
+      </c>
+      <c r="C43">
+        <v>400.08800000000002</v>
+      </c>
+      <c r="D43">
+        <v>336.90499999999997</v>
+      </c>
+      <c r="E43">
+        <v>400.12299999999999</v>
+      </c>
+      <c r="F43">
+        <v>336.90100000000001</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>365.95220000000006</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>1.6794733291417507</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>156.13399999999999</v>
+      </c>
+      <c r="C46">
+        <v>163.673</v>
+      </c>
+      <c r="D46">
+        <v>156.11699999999999</v>
+      </c>
+      <c r="E46">
+        <v>156.16499999999999</v>
+      </c>
+      <c r="F46">
+        <v>160.03399999999999</v>
+      </c>
+      <c r="G46">
+        <f>AVERAGE(B46:F46)</f>
+        <v>158.4246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47">
+        <v>139.14400000000001</v>
+      </c>
+      <c r="C47">
+        <v>139.16399999999999</v>
+      </c>
+      <c r="D47">
+        <v>140.739</v>
+      </c>
+      <c r="E47">
+        <v>136.191</v>
+      </c>
+      <c r="F47">
+        <v>133.333</v>
+      </c>
+      <c r="G47">
+        <f>AVERAGE(B47:F47)</f>
+        <v>137.71420000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48">
+        <v>112.265</v>
+      </c>
+      <c r="C48">
+        <v>110.349</v>
+      </c>
+      <c r="D48">
+        <v>112.289</v>
+      </c>
+      <c r="E48">
+        <v>110.358</v>
+      </c>
+      <c r="F48">
+        <v>110.352</v>
+      </c>
+      <c r="G48">
+        <f>AVERAGE(B48:F48)</f>
+        <v>111.12260000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>44</v>
       </c>
-      <c r="B17">
-        <v>84.192999999999998</v>
-      </c>
-      <c r="C17">
-        <v>63.304099999999998</v>
-      </c>
-      <c r="D17">
-        <v>80</v>
-      </c>
-      <c r="E17">
-        <v>78</v>
-      </c>
-      <c r="F17">
-        <v>82.345399999999998</v>
-      </c>
-      <c r="G17">
-        <v>84.139700000000005</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18">
-        <v>99.204300000000003</v>
-      </c>
-      <c r="C18">
-        <v>70.402500000000003</v>
-      </c>
-      <c r="D18">
-        <v>92</v>
-      </c>
-      <c r="E18">
-        <v>89</v>
-      </c>
-      <c r="F18">
-        <v>79.364999999999995</v>
-      </c>
-      <c r="G18">
-        <v>95.824799999999996</v>
+      <c r="B49">
+        <v>96.973500000000001</v>
+      </c>
+      <c r="C49">
+        <v>99.879599999999996</v>
+      </c>
+      <c r="D49">
+        <v>99.982100000000003</v>
+      </c>
+      <c r="E49">
+        <v>98.472200000000001</v>
+      </c>
+      <c r="F49">
+        <v>98.465000000000003</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49:G61" si="2">AVERAGE(B49:F49)</f>
+        <v>98.754479999999987</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50">
+        <v>71.903599999999997</v>
+      </c>
+      <c r="C50">
+        <v>71.912400000000005</v>
+      </c>
+      <c r="D50">
+        <v>71.113299999999995</v>
+      </c>
+      <c r="E50">
+        <v>71.1126</v>
+      </c>
+      <c r="F50">
+        <v>69.573400000000007</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>71.123059999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51">
+        <v>59.816600000000001</v>
+      </c>
+      <c r="C51">
+        <v>59.260800000000003</v>
+      </c>
+      <c r="D51">
+        <v>59.814900000000002</v>
+      </c>
+      <c r="E51">
+        <v>59.817300000000003</v>
+      </c>
+      <c r="F51">
+        <v>59.816400000000002</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>59.705200000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52">
+        <v>55.909199999999998</v>
+      </c>
+      <c r="C52">
+        <v>55.175600000000003</v>
+      </c>
+      <c r="D52">
+        <v>55.1753</v>
+      </c>
+      <c r="E52">
+        <v>55.625799999999998</v>
+      </c>
+      <c r="F52">
+        <v>55.092500000000001</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>55.395679999999992</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53">
+        <v>56.638500000000001</v>
+      </c>
+      <c r="C53">
+        <v>55.653399999999998</v>
+      </c>
+      <c r="D53">
+        <v>57.144300000000001</v>
+      </c>
+      <c r="E53">
+        <v>57.349899999999998</v>
+      </c>
+      <c r="F53">
+        <v>57.145400000000002</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="2"/>
+        <v>56.786299999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54">
+        <v>58.716799999999999</v>
+      </c>
+      <c r="C54">
+        <v>58.716999999999999</v>
+      </c>
+      <c r="D54">
+        <v>59.2637</v>
+      </c>
+      <c r="E54">
+        <v>58.718699999999998</v>
+      </c>
+      <c r="F54">
+        <v>58.7166</v>
+      </c>
+      <c r="G54">
+        <f>AVERAGE(B54:F54)</f>
+        <v>58.826559999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55">
+        <v>83.1434</v>
+      </c>
+      <c r="C55">
+        <v>84.212199999999996</v>
+      </c>
+      <c r="D55">
+        <v>84.221299999999999</v>
+      </c>
+      <c r="E55">
+        <v>84.211699999999993</v>
+      </c>
+      <c r="F55">
+        <v>82.052899999999994</v>
+      </c>
+      <c r="G55">
+        <f>AVERAGE(B55:F55)</f>
+        <v>83.568299999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56">
+        <v>100.515</v>
+      </c>
+      <c r="C56">
+        <v>101.59699999999999</v>
+      </c>
+      <c r="D56">
+        <v>100.006</v>
+      </c>
+      <c r="E56">
+        <v>101.589</v>
+      </c>
+      <c r="F56">
+        <v>98.503299999999996</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="2"/>
+        <v>100.44206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57">
+        <v>133.35900000000001</v>
+      </c>
+      <c r="C57">
+        <v>136.18600000000001</v>
+      </c>
+      <c r="D57">
+        <v>134.90600000000001</v>
+      </c>
+      <c r="E57">
+        <v>136.17099999999999</v>
+      </c>
+      <c r="F57">
+        <v>133.358</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="2"/>
+        <v>134.79599999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58">
+        <v>181.01300000000001</v>
+      </c>
+      <c r="C58">
+        <v>177.79</v>
+      </c>
+      <c r="D58">
+        <v>177.78899999999999</v>
+      </c>
+      <c r="E58">
+        <v>172.99700000000001</v>
+      </c>
+      <c r="F58">
+        <v>177.815</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>177.48079999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59">
+        <v>228.62700000000001</v>
+      </c>
+      <c r="C59">
+        <v>237.26400000000001</v>
+      </c>
+      <c r="D59">
+        <v>229.24299999999999</v>
+      </c>
+      <c r="E59">
+        <v>246.13200000000001</v>
+      </c>
+      <c r="F59">
+        <v>220.72800000000001</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="2"/>
+        <v>232.39880000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60">
+        <v>213.38</v>
+      </c>
+      <c r="C60">
+        <v>213.34700000000001</v>
+      </c>
+      <c r="D60">
+        <v>213.386</v>
+      </c>
+      <c r="E60">
+        <v>213.393</v>
+      </c>
+      <c r="F60">
+        <v>208.571</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="2"/>
+        <v>212.41540000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61">
+        <v>220.75800000000001</v>
+      </c>
+      <c r="C61">
+        <v>220.77600000000001</v>
+      </c>
+      <c r="D61">
+        <v>220.71799999999999</v>
+      </c>
+      <c r="E61">
+        <v>220.71600000000001</v>
+      </c>
+      <c r="F61">
+        <v>206.517</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>217.89699999999999</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A126:G144">
+    <sortCondition ref="A126"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B27:F27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Added more perf numbers for Atomix
</commit_message>
<xml_diff>
--- a/code/WiFi/Performance.xlsx
+++ b/code/WiFi/Performance.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Old" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="151">
   <si>
     <t>test_scramble_perf</t>
   </si>
@@ -462,6 +463,24 @@
   </si>
   <si>
     <t>2Th/1Th</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>1-thread</t>
+  </si>
+  <si>
+    <t>2-thread-optimal</t>
+  </si>
+  <si>
+    <t>2-thread-old</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Eyal's numbers:</t>
   </si>
 </sst>
 </file>
@@ -3859,10 +3878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77:D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +4373,7 @@
         <v>185.09740000000002</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:H43" si="0">$G29/$G47</f>
+        <f>$G29/$G47</f>
         <v>1.3440690938189381</v>
       </c>
     </row>
@@ -4382,7 +4401,7 @@
         <v>139.845</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H29:H43" si="0">$G30/$G48</f>
         <v>1.2584748736980595</v>
       </c>
     </row>
@@ -5132,6 +5151,263 @@
       <c r="G61">
         <f t="shared" si="2"/>
         <v>217.89699999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>71.962000000000003</v>
+      </c>
+      <c r="D67">
+        <v>120.77</v>
+      </c>
+      <c r="H67">
+        <v>96.225999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>65.054000000000002</v>
+      </c>
+      <c r="D68">
+        <v>110.726</v>
+      </c>
+      <c r="H68">
+        <v>90.411000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="B69">
+        <v>54.067</v>
+      </c>
+      <c r="D69">
+        <v>89.581999999999994</v>
+      </c>
+      <c r="H69">
+        <v>83.775999999999996</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>18</v>
+      </c>
+      <c r="B70">
+        <v>48.688000000000002</v>
+      </c>
+      <c r="D70">
+        <v>74.278000000000006</v>
+      </c>
+      <c r="H70">
+        <v>73.936999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>24</v>
+      </c>
+      <c r="B71">
+        <v>36.741</v>
+      </c>
+      <c r="D71">
+        <v>63.968000000000004</v>
+      </c>
+      <c r="H71">
+        <v>62.466999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>36</v>
+      </c>
+      <c r="B72">
+        <v>31.670999999999999</v>
+      </c>
+      <c r="D72">
+        <v>50.856999999999999</v>
+      </c>
+      <c r="H72">
+        <v>50.816000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>48</v>
+      </c>
+      <c r="B73">
+        <v>28.651</v>
+      </c>
+      <c r="D73">
+        <v>46.414999999999999</v>
+      </c>
+      <c r="H73">
+        <v>42.634999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>54</v>
+      </c>
+      <c r="B74">
+        <v>25.201000000000001</v>
+      </c>
+      <c r="D74">
+        <v>50.433</v>
+      </c>
+      <c r="H74">
+        <v>38.588000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>6</v>
+      </c>
+      <c r="B77">
+        <v>29.245000000000001</v>
+      </c>
+      <c r="D77">
+        <v>35.978999999999999</v>
+      </c>
+      <c r="H77">
+        <v>32.814</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>9</v>
+      </c>
+      <c r="B78">
+        <v>43.296999999999997</v>
+      </c>
+      <c r="D78">
+        <v>56.683</v>
+      </c>
+      <c r="H78">
+        <v>50.832000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>12</v>
+      </c>
+      <c r="B79">
+        <v>51.829000000000001</v>
+      </c>
+      <c r="D79">
+        <v>74.492999999999995</v>
+      </c>
+      <c r="H79">
+        <v>60.854999999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>18</v>
+      </c>
+      <c r="B80">
+        <v>74.122</v>
+      </c>
+      <c r="D80">
+        <v>110.402</v>
+      </c>
+      <c r="H80">
+        <v>96.483000000000004</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>24</v>
+      </c>
+      <c r="B81">
+        <v>94.540999999999997</v>
+      </c>
+      <c r="D81">
+        <v>149.12799999999999</v>
+      </c>
+      <c r="H81">
+        <v>125.709</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>36</v>
+      </c>
+      <c r="B82">
+        <v>108.226</v>
+      </c>
+      <c r="D82">
+        <v>197.30799999999999</v>
+      </c>
+      <c r="H82">
+        <v>189.06700000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>48</v>
+      </c>
+      <c r="B83">
+        <v>109.64100000000001</v>
+      </c>
+      <c r="D83">
+        <v>193.47200000000001</v>
+      </c>
+      <c r="H83">
+        <v>191.03299999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>54</v>
+      </c>
+      <c r="B84">
+        <v>125.764</v>
+      </c>
+      <c r="D84">
+        <v>205.67599999999999</v>
+      </c>
+      <c r="H84">
+        <v>195.65299999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>